<commit_message>
Add 2 questions about max and min speed and temp to SIQ
</commit_message>
<xml_diff>
--- a/Digital_Air_Conditional_Screen/Project Managment/Review Log Sheet/Review Log Sheet.xlsx
+++ b/Digital_Air_Conditional_Screen/Project Managment/Review Log Sheet/Review Log Sheet.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="44">
   <si>
     <t>Project Name:</t>
   </si>
@@ -140,6 +140,18 @@
   </si>
   <si>
     <t>17/3/2016</t>
+  </si>
+  <si>
+    <t>Rev_02_03</t>
+  </si>
+  <si>
+    <t>Low</t>
+  </si>
+  <si>
+    <t>Add Code folders</t>
+  </si>
+  <si>
+    <t>Reviewer</t>
   </si>
 </sst>
 </file>
@@ -262,31 +274,31 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="14" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -569,10 +581,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C1:T15"/>
+  <dimension ref="C1:U15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="R10" sqref="R10:S10"/>
+    <sheetView tabSelected="1" topLeftCell="JS1" workbookViewId="0">
+      <selection activeCell="U6" sqref="U6:U13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -582,432 +594,444 @@
     <col min="12" max="12" width="10.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="3:20" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="2" spans="3:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C2" s="7" t="s">
+    <row r="1" spans="3:21" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="2" spans="3:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C2" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="8"/>
-      <c r="E2" s="4" t="s">
+      <c r="D2" s="12"/>
+      <c r="E2" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="F2" s="5"/>
-    </row>
-    <row r="3" spans="3:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C3" s="7" t="s">
+      <c r="F2" s="10"/>
+    </row>
+    <row r="3" spans="3:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C3" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="8"/>
-      <c r="E3" s="4" t="s">
+      <c r="D3" s="12"/>
+      <c r="E3" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="F3" s="5"/>
-    </row>
-    <row r="4" spans="3:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="F3" s="10"/>
+    </row>
+    <row r="4" spans="3:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C4" s="2"/>
       <c r="D4" s="2"/>
       <c r="E4" s="2"/>
       <c r="F4" s="2"/>
     </row>
-    <row r="5" spans="3:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C5" s="6" t="s">
+    <row r="5" spans="3:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C5" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="D5" s="6"/>
-      <c r="E5" s="6" t="s">
+      <c r="D5" s="8"/>
+      <c r="E5" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="F5" s="6"/>
-      <c r="G5" s="6" t="s">
+      <c r="F5" s="8"/>
+      <c r="G5" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="H5" s="6"/>
-      <c r="I5" s="6"/>
-      <c r="J5" s="6" t="s">
+      <c r="H5" s="8"/>
+      <c r="I5" s="8"/>
+      <c r="J5" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="K5" s="6"/>
-      <c r="L5" s="6"/>
-      <c r="M5" s="6" t="s">
+      <c r="K5" s="8"/>
+      <c r="L5" s="8"/>
+      <c r="M5" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="N5" s="6"/>
-      <c r="O5" s="6"/>
-      <c r="P5" s="6" t="s">
+      <c r="N5" s="8"/>
+      <c r="O5" s="8"/>
+      <c r="P5" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="Q5" s="6"/>
-      <c r="R5" s="6" t="s">
+      <c r="Q5" s="8"/>
+      <c r="R5" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="S5" s="6"/>
+      <c r="S5" s="8"/>
       <c r="T5" s="3" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="6" spans="3:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C6" s="9" t="s">
+      <c r="U5" s="3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="6" spans="3:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C6" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="D6" s="9"/>
-      <c r="E6" s="10" t="s">
+      <c r="D6" s="5"/>
+      <c r="E6" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="F6" s="10"/>
-      <c r="G6" s="9" t="s">
+      <c r="F6" s="7"/>
+      <c r="G6" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="H6" s="9"/>
-      <c r="I6" s="9"/>
-      <c r="J6" s="9" t="s">
+      <c r="H6" s="5"/>
+      <c r="I6" s="5"/>
+      <c r="J6" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="K6" s="9"/>
-      <c r="L6" s="9"/>
-      <c r="M6" s="9" t="s">
+      <c r="K6" s="5"/>
+      <c r="L6" s="5"/>
+      <c r="M6" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="N6" s="9"/>
-      <c r="O6" s="9"/>
-      <c r="P6" s="12">
+      <c r="N6" s="5"/>
+      <c r="O6" s="5"/>
+      <c r="P6" s="4">
         <v>42707</v>
       </c>
-      <c r="Q6" s="9"/>
-      <c r="R6" s="12" t="s">
+      <c r="Q6" s="5"/>
+      <c r="R6" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="S6" s="9"/>
+      <c r="S6" s="5"/>
       <c r="T6" s="1" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="7" spans="3:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C7" s="9" t="s">
+      <c r="U6" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="7" spans="3:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C7" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="D7" s="9"/>
-      <c r="E7" s="11" t="s">
+      <c r="D7" s="5"/>
+      <c r="E7" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="F7" s="11"/>
-      <c r="G7" s="9" t="s">
+      <c r="F7" s="6"/>
+      <c r="G7" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="H7" s="9"/>
-      <c r="I7" s="9"/>
-      <c r="J7" s="9" t="s">
+      <c r="H7" s="5"/>
+      <c r="I7" s="5"/>
+      <c r="J7" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="K7" s="9"/>
-      <c r="L7" s="9"/>
-      <c r="M7" s="9" t="s">
+      <c r="K7" s="5"/>
+      <c r="L7" s="5"/>
+      <c r="M7" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="N7" s="9"/>
-      <c r="O7" s="9"/>
-      <c r="P7" s="12">
+      <c r="N7" s="5"/>
+      <c r="O7" s="5"/>
+      <c r="P7" s="4">
         <v>42707</v>
       </c>
-      <c r="Q7" s="9"/>
-      <c r="R7" s="12" t="s">
+      <c r="Q7" s="5"/>
+      <c r="R7" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="S7" s="9"/>
+      <c r="S7" s="5"/>
       <c r="T7" s="1" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="8" spans="3:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C8" s="9" t="s">
+      <c r="U7" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="8" spans="3:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C8" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="D8" s="9"/>
-      <c r="E8" s="11" t="s">
+      <c r="D8" s="5"/>
+      <c r="E8" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="F8" s="11"/>
-      <c r="G8" s="9" t="s">
+      <c r="F8" s="6"/>
+      <c r="G8" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="H8" s="9"/>
-      <c r="I8" s="9"/>
-      <c r="J8" s="9" t="s">
+      <c r="H8" s="5"/>
+      <c r="I8" s="5"/>
+      <c r="J8" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="K8" s="9"/>
-      <c r="L8" s="9"/>
-      <c r="M8" s="9" t="s">
+      <c r="K8" s="5"/>
+      <c r="L8" s="5"/>
+      <c r="M8" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="N8" s="9"/>
-      <c r="O8" s="9"/>
-      <c r="P8" s="12">
+      <c r="N8" s="5"/>
+      <c r="O8" s="5"/>
+      <c r="P8" s="4">
         <v>42707</v>
       </c>
-      <c r="Q8" s="9"/>
-      <c r="R8" s="12">
+      <c r="Q8" s="5"/>
+      <c r="R8" s="4">
         <v>42707</v>
       </c>
-      <c r="S8" s="9"/>
+      <c r="S8" s="5"/>
       <c r="T8" s="1" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="9" spans="3:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C9" s="9" t="s">
+      <c r="U8" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="9" spans="3:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C9" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="D9" s="9"/>
-      <c r="E9" s="11" t="s">
+      <c r="D9" s="5"/>
+      <c r="E9" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="F9" s="11"/>
-      <c r="G9" s="9" t="s">
+      <c r="F9" s="6"/>
+      <c r="G9" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="H9" s="9"/>
-      <c r="I9" s="9"/>
-      <c r="J9" s="9" t="s">
+      <c r="H9" s="5"/>
+      <c r="I9" s="5"/>
+      <c r="J9" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="K9" s="9"/>
-      <c r="L9" s="9"/>
-      <c r="M9" s="9" t="s">
+      <c r="K9" s="5"/>
+      <c r="L9" s="5"/>
+      <c r="M9" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="N9" s="9"/>
-      <c r="O9" s="9"/>
-      <c r="P9" s="12">
+      <c r="N9" s="5"/>
+      <c r="O9" s="5"/>
+      <c r="P9" s="4">
         <v>42707</v>
       </c>
-      <c r="Q9" s="9"/>
-      <c r="R9" s="12" t="s">
+      <c r="Q9" s="5"/>
+      <c r="R9" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="S9" s="9"/>
+      <c r="S9" s="5"/>
       <c r="T9" s="1" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="10" spans="3:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C10" s="9" t="s">
+      <c r="U9" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="10" spans="3:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C10" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="D10" s="9"/>
-      <c r="E10" s="10" t="s">
+      <c r="D10" s="5"/>
+      <c r="E10" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="F10" s="10"/>
-      <c r="G10" s="9" t="s">
+      <c r="F10" s="7"/>
+      <c r="G10" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="H10" s="9"/>
-      <c r="I10" s="9"/>
-      <c r="J10" s="9" t="s">
+      <c r="H10" s="5"/>
+      <c r="I10" s="5"/>
+      <c r="J10" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="K10" s="9"/>
-      <c r="L10" s="9"/>
-      <c r="M10" s="9" t="s">
+      <c r="K10" s="5"/>
+      <c r="L10" s="5"/>
+      <c r="M10" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="N10" s="9"/>
-      <c r="O10" s="9"/>
-      <c r="P10" s="12">
+      <c r="N10" s="5"/>
+      <c r="O10" s="5"/>
+      <c r="P10" s="4">
         <v>42707</v>
       </c>
-      <c r="Q10" s="9"/>
-      <c r="R10" s="12" t="s">
+      <c r="Q10" s="5"/>
+      <c r="R10" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="S10" s="9"/>
+      <c r="S10" s="5"/>
       <c r="T10" s="1" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="11" spans="3:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C11" s="9" t="s">
+      <c r="U10" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="11" spans="3:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C11" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="D11" s="9"/>
-      <c r="E11" s="11" t="s">
+      <c r="D11" s="5"/>
+      <c r="E11" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="F11" s="11"/>
-      <c r="G11" s="9" t="s">
+      <c r="F11" s="6"/>
+      <c r="G11" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="H11" s="9"/>
-      <c r="I11" s="9"/>
-      <c r="J11" s="9" t="s">
+      <c r="H11" s="5"/>
+      <c r="I11" s="5"/>
+      <c r="J11" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="K11" s="9"/>
-      <c r="L11" s="9"/>
-      <c r="M11" s="9" t="s">
+      <c r="K11" s="5"/>
+      <c r="L11" s="5"/>
+      <c r="M11" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="N11" s="9"/>
-      <c r="O11" s="9"/>
-      <c r="P11" s="12">
+      <c r="N11" s="5"/>
+      <c r="O11" s="5"/>
+      <c r="P11" s="4">
         <v>42707</v>
       </c>
-      <c r="Q11" s="9"/>
-      <c r="R11" s="9" t="s">
+      <c r="Q11" s="5"/>
+      <c r="R11" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="S11" s="9"/>
+      <c r="S11" s="5"/>
       <c r="T11" s="1" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="12" spans="3:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C12" s="9" t="s">
+      <c r="U11" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="12" spans="3:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C12" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="D12" s="9"/>
-      <c r="E12" s="10" t="s">
+      <c r="D12" s="5"/>
+      <c r="E12" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="F12" s="10"/>
-      <c r="G12" s="9" t="s">
+      <c r="F12" s="7"/>
+      <c r="G12" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="H12" s="9"/>
-      <c r="I12" s="9"/>
-      <c r="J12" s="9" t="s">
+      <c r="H12" s="5"/>
+      <c r="I12" s="5"/>
+      <c r="J12" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="K12" s="9"/>
-      <c r="L12" s="9"/>
-      <c r="M12" s="9" t="s">
+      <c r="K12" s="5"/>
+      <c r="L12" s="5"/>
+      <c r="M12" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="N12" s="9"/>
-      <c r="O12" s="9"/>
-      <c r="P12" s="12">
+      <c r="N12" s="5"/>
+      <c r="O12" s="5"/>
+      <c r="P12" s="4">
         <v>42707</v>
       </c>
-      <c r="Q12" s="9"/>
-      <c r="R12" s="9" t="s">
+      <c r="Q12" s="5"/>
+      <c r="R12" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="S12" s="9"/>
+      <c r="S12" s="5"/>
       <c r="T12" s="1" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="13" spans="3:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C13" s="9"/>
-      <c r="D13" s="9"/>
-      <c r="E13" s="9"/>
-      <c r="F13" s="9"/>
-      <c r="G13" s="9"/>
-      <c r="H13" s="9"/>
-      <c r="I13" s="9"/>
-      <c r="J13" s="9"/>
-      <c r="K13" s="9"/>
-      <c r="L13" s="9"/>
-      <c r="M13" s="9"/>
-      <c r="N13" s="9"/>
-      <c r="O13" s="9"/>
-      <c r="P13" s="9"/>
-      <c r="Q13" s="9"/>
-      <c r="R13" s="9"/>
-      <c r="S13" s="9"/>
-      <c r="T13" s="1"/>
-    </row>
-    <row r="14" spans="3:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C14" s="9"/>
-      <c r="D14" s="9"/>
-      <c r="E14" s="9"/>
-      <c r="F14" s="9"/>
-      <c r="G14" s="9"/>
-      <c r="H14" s="9"/>
-      <c r="I14" s="9"/>
-      <c r="J14" s="9"/>
-      <c r="K14" s="9"/>
-      <c r="L14" s="9"/>
-      <c r="M14" s="9"/>
-      <c r="N14" s="9"/>
-      <c r="O14" s="9"/>
-      <c r="P14" s="9"/>
-      <c r="Q14" s="9"/>
-      <c r="R14" s="9"/>
-      <c r="S14" s="9"/>
+      <c r="U12" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="13" spans="3:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C13" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="D13" s="5"/>
+      <c r="E13" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="F13" s="5"/>
+      <c r="G13" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="H13" s="5"/>
+      <c r="I13" s="5"/>
+      <c r="J13" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="K13" s="5"/>
+      <c r="L13" s="5"/>
+      <c r="M13" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="N13" s="5"/>
+      <c r="O13" s="5"/>
+      <c r="P13" s="4">
+        <v>42404</v>
+      </c>
+      <c r="Q13" s="5"/>
+      <c r="R13" s="4">
+        <v>42433</v>
+      </c>
+      <c r="S13" s="5"/>
+      <c r="T13" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="U13" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="14" spans="3:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C14" s="5"/>
+      <c r="D14" s="5"/>
+      <c r="E14" s="5"/>
+      <c r="F14" s="5"/>
+      <c r="G14" s="5"/>
+      <c r="H14" s="5"/>
+      <c r="I14" s="5"/>
+      <c r="J14" s="5"/>
+      <c r="K14" s="5"/>
+      <c r="L14" s="5"/>
+      <c r="M14" s="5"/>
+      <c r="N14" s="5"/>
+      <c r="O14" s="5"/>
+      <c r="P14" s="5"/>
+      <c r="Q14" s="5"/>
+      <c r="R14" s="5"/>
+      <c r="S14" s="5"/>
       <c r="T14" s="1"/>
-    </row>
-    <row r="15" spans="3:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C15" s="9"/>
-      <c r="D15" s="9"/>
-      <c r="E15" s="9"/>
-      <c r="F15" s="9"/>
-      <c r="G15" s="9"/>
-      <c r="H15" s="9"/>
-      <c r="I15" s="9"/>
-      <c r="J15" s="9"/>
-      <c r="K15" s="9"/>
-      <c r="L15" s="9"/>
-      <c r="M15" s="9"/>
-      <c r="N15" s="9"/>
-      <c r="O15" s="9"/>
-      <c r="P15" s="9"/>
-      <c r="Q15" s="9"/>
-      <c r="R15" s="9"/>
-      <c r="S15" s="9"/>
+      <c r="U14" s="1"/>
+    </row>
+    <row r="15" spans="3:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C15" s="5"/>
+      <c r="D15" s="5"/>
+      <c r="E15" s="5"/>
+      <c r="F15" s="5"/>
+      <c r="G15" s="5"/>
+      <c r="H15" s="5"/>
+      <c r="I15" s="5"/>
+      <c r="J15" s="5"/>
+      <c r="K15" s="5"/>
+      <c r="L15" s="5"/>
+      <c r="M15" s="5"/>
+      <c r="N15" s="5"/>
+      <c r="O15" s="5"/>
+      <c r="P15" s="5"/>
+      <c r="Q15" s="5"/>
+      <c r="R15" s="5"/>
+      <c r="S15" s="5"/>
       <c r="T15" s="1"/>
+      <c r="U15" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="81">
-    <mergeCell ref="P11:Q11"/>
-    <mergeCell ref="P12:Q12"/>
-    <mergeCell ref="P13:Q13"/>
-    <mergeCell ref="P14:Q14"/>
-    <mergeCell ref="P15:Q15"/>
-    <mergeCell ref="R11:S11"/>
-    <mergeCell ref="R12:S12"/>
-    <mergeCell ref="R13:S13"/>
-    <mergeCell ref="R14:S14"/>
-    <mergeCell ref="R15:S15"/>
-    <mergeCell ref="G13:I13"/>
-    <mergeCell ref="J13:L13"/>
-    <mergeCell ref="J14:L14"/>
-    <mergeCell ref="J15:L15"/>
-    <mergeCell ref="M11:O11"/>
-    <mergeCell ref="M12:O12"/>
-    <mergeCell ref="M13:O13"/>
-    <mergeCell ref="M14:O14"/>
-    <mergeCell ref="M15:O15"/>
-    <mergeCell ref="J12:L12"/>
-    <mergeCell ref="C12:D12"/>
-    <mergeCell ref="C13:D13"/>
-    <mergeCell ref="C14:D14"/>
-    <mergeCell ref="C15:D15"/>
-    <mergeCell ref="E11:F11"/>
-    <mergeCell ref="E12:F12"/>
-    <mergeCell ref="C11:D11"/>
-    <mergeCell ref="E13:F13"/>
-    <mergeCell ref="P6:Q6"/>
-    <mergeCell ref="P7:Q7"/>
-    <mergeCell ref="P8:Q8"/>
-    <mergeCell ref="P9:Q9"/>
-    <mergeCell ref="P10:Q10"/>
-    <mergeCell ref="J11:L11"/>
-    <mergeCell ref="J9:L9"/>
-    <mergeCell ref="M9:O9"/>
-    <mergeCell ref="J10:L10"/>
-    <mergeCell ref="M10:O10"/>
-    <mergeCell ref="R6:S6"/>
-    <mergeCell ref="R7:S7"/>
-    <mergeCell ref="R8:S8"/>
-    <mergeCell ref="R9:S9"/>
-    <mergeCell ref="R10:S10"/>
-    <mergeCell ref="J6:L6"/>
-    <mergeCell ref="M6:O6"/>
-    <mergeCell ref="J7:L7"/>
-    <mergeCell ref="M7:O7"/>
-    <mergeCell ref="J8:L8"/>
-    <mergeCell ref="M8:O8"/>
+    <mergeCell ref="E2:F2"/>
+    <mergeCell ref="E3:F3"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="G5:I5"/>
+    <mergeCell ref="J5:L5"/>
+    <mergeCell ref="M5:O5"/>
+    <mergeCell ref="P5:Q5"/>
+    <mergeCell ref="R5:S5"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="C7:D7"/>
+    <mergeCell ref="C8:D8"/>
+    <mergeCell ref="C9:D9"/>
+    <mergeCell ref="C10:D10"/>
     <mergeCell ref="G6:I6"/>
     <mergeCell ref="G7:I7"/>
     <mergeCell ref="E14:F14"/>
@@ -1024,22 +1048,55 @@
     <mergeCell ref="G14:I14"/>
     <mergeCell ref="G15:I15"/>
     <mergeCell ref="G12:I12"/>
-    <mergeCell ref="C6:D6"/>
-    <mergeCell ref="C7:D7"/>
-    <mergeCell ref="C8:D8"/>
-    <mergeCell ref="C9:D9"/>
-    <mergeCell ref="C10:D10"/>
-    <mergeCell ref="G5:I5"/>
-    <mergeCell ref="J5:L5"/>
-    <mergeCell ref="M5:O5"/>
-    <mergeCell ref="P5:Q5"/>
-    <mergeCell ref="R5:S5"/>
-    <mergeCell ref="E2:F2"/>
-    <mergeCell ref="E3:F3"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="C2:D2"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="J9:L9"/>
+    <mergeCell ref="M9:O9"/>
+    <mergeCell ref="J10:L10"/>
+    <mergeCell ref="M10:O10"/>
+    <mergeCell ref="R6:S6"/>
+    <mergeCell ref="R7:S7"/>
+    <mergeCell ref="R8:S8"/>
+    <mergeCell ref="R9:S9"/>
+    <mergeCell ref="R10:S10"/>
+    <mergeCell ref="J6:L6"/>
+    <mergeCell ref="M6:O6"/>
+    <mergeCell ref="J7:L7"/>
+    <mergeCell ref="M7:O7"/>
+    <mergeCell ref="J8:L8"/>
+    <mergeCell ref="M8:O8"/>
+    <mergeCell ref="P6:Q6"/>
+    <mergeCell ref="P7:Q7"/>
+    <mergeCell ref="P8:Q8"/>
+    <mergeCell ref="P9:Q9"/>
+    <mergeCell ref="P10:Q10"/>
+    <mergeCell ref="C12:D12"/>
+    <mergeCell ref="C13:D13"/>
+    <mergeCell ref="C14:D14"/>
+    <mergeCell ref="C15:D15"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="E12:F12"/>
+    <mergeCell ref="C11:D11"/>
+    <mergeCell ref="E13:F13"/>
+    <mergeCell ref="G13:I13"/>
+    <mergeCell ref="J13:L13"/>
+    <mergeCell ref="J14:L14"/>
+    <mergeCell ref="J15:L15"/>
+    <mergeCell ref="M11:O11"/>
+    <mergeCell ref="M12:O12"/>
+    <mergeCell ref="M13:O13"/>
+    <mergeCell ref="M14:O14"/>
+    <mergeCell ref="M15:O15"/>
+    <mergeCell ref="J12:L12"/>
+    <mergeCell ref="J11:L11"/>
+    <mergeCell ref="R11:S11"/>
+    <mergeCell ref="R12:S12"/>
+    <mergeCell ref="R13:S13"/>
+    <mergeCell ref="R14:S14"/>
+    <mergeCell ref="R15:S15"/>
+    <mergeCell ref="P11:Q11"/>
+    <mergeCell ref="P12:Q12"/>
+    <mergeCell ref="P13:Q13"/>
+    <mergeCell ref="P14:Q14"/>
+    <mergeCell ref="P15:Q15"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Add Folders in CI Add New info in CRS Add New Req. in SRS Add New Q in SIQ Add Interactive between Layers Add Tags in CDDs Add new Test Cases
</commit_message>
<xml_diff>
--- a/Digital_Air_Conditional_Screen/Project Managment/Review Log Sheet/Review Log Sheet.xlsx
+++ b/Digital_Air_Conditional_Screen/Project Managment/Review Log Sheet/Review Log Sheet.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="153222"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16668" windowHeight="7728"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21960" windowHeight="7728"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="69">
   <si>
     <t>Project Name:</t>
   </si>
@@ -152,6 +152,81 @@
   </si>
   <si>
     <t>Reviewer</t>
+  </si>
+  <si>
+    <t>Rev_02_05</t>
+  </si>
+  <si>
+    <t>Rev_02_06</t>
+  </si>
+  <si>
+    <t>Rev_02_07</t>
+  </si>
+  <si>
+    <t>Rev_02_08</t>
+  </si>
+  <si>
+    <t>Rev_02_09</t>
+  </si>
+  <si>
+    <t>Rev_02_10</t>
+  </si>
+  <si>
+    <t>RTM</t>
+  </si>
+  <si>
+    <t>Rev_04_04</t>
+  </si>
+  <si>
+    <t>Make connection between Tags</t>
+  </si>
+  <si>
+    <t>Hadir</t>
+  </si>
+  <si>
+    <t>SRS</t>
+  </si>
+  <si>
+    <t>SIQ</t>
+  </si>
+  <si>
+    <t>HLD</t>
+  </si>
+  <si>
+    <t>Add more information about project</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Add new requirement </t>
+  </si>
+  <si>
+    <t>Add quistion about rang of Speed &amp;Temp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Add interactive between Layers </t>
+  </si>
+  <si>
+    <t>Test Cases</t>
+  </si>
+  <si>
+    <t>Add new Test Cases with tags</t>
+  </si>
+  <si>
+    <t>CDD LCD</t>
+  </si>
+  <si>
+    <t>Add Tags</t>
+  </si>
+  <si>
+    <t>Rev_02_11</t>
+  </si>
+  <si>
+    <t>CDD DIO</t>
+  </si>
+  <si>
+    <t>CDD EEPROM</t>
+  </si>
+  <si>
+    <t>CDD TS</t>
   </si>
 </sst>
 </file>
@@ -274,31 +349,31 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="14" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -581,39 +656,40 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C1:U15"/>
+  <dimension ref="C1:U29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="JS1" workbookViewId="0">
-      <selection activeCell="U6" sqref="U6:U13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J25" sqref="J25:L25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="5" max="5" width="13" customWidth="1"/>
     <col min="6" max="6" width="13.21875" customWidth="1"/>
-    <col min="12" max="12" width="10.33203125" customWidth="1"/>
+    <col min="11" max="11" width="14.109375" customWidth="1"/>
+    <col min="12" max="12" width="15.77734375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="3:21" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="3:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C2" s="11" t="s">
+      <c r="C2" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="12"/>
-      <c r="E2" s="9" t="s">
+      <c r="D2" s="8"/>
+      <c r="E2" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="F2" s="10"/>
+      <c r="F2" s="5"/>
     </row>
     <row r="3" spans="3:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C3" s="11" t="s">
+      <c r="C3" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="12"/>
-      <c r="E3" s="9" t="s">
+      <c r="D3" s="8"/>
+      <c r="E3" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="F3" s="10"/>
+      <c r="F3" s="5"/>
     </row>
     <row r="4" spans="3:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C4" s="2"/>
@@ -622,37 +698,37 @@
       <c r="F4" s="2"/>
     </row>
     <row r="5" spans="3:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C5" s="8" t="s">
+      <c r="C5" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="D5" s="8"/>
-      <c r="E5" s="8" t="s">
+      <c r="D5" s="6"/>
+      <c r="E5" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="F5" s="8"/>
-      <c r="G5" s="8" t="s">
+      <c r="F5" s="6"/>
+      <c r="G5" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="H5" s="8"/>
-      <c r="I5" s="8"/>
-      <c r="J5" s="8" t="s">
+      <c r="H5" s="6"/>
+      <c r="I5" s="6"/>
+      <c r="J5" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="K5" s="8"/>
-      <c r="L5" s="8"/>
-      <c r="M5" s="8" t="s">
+      <c r="K5" s="6"/>
+      <c r="L5" s="6"/>
+      <c r="M5" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="N5" s="8"/>
-      <c r="O5" s="8"/>
-      <c r="P5" s="8" t="s">
+      <c r="N5" s="6"/>
+      <c r="O5" s="6"/>
+      <c r="P5" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="Q5" s="8"/>
-      <c r="R5" s="8" t="s">
+      <c r="Q5" s="6"/>
+      <c r="R5" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="S5" s="8"/>
+      <c r="S5" s="6"/>
       <c r="T5" s="3" t="s">
         <v>36</v>
       </c>
@@ -661,37 +737,37 @@
       </c>
     </row>
     <row r="6" spans="3:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C6" s="5" t="s">
+      <c r="C6" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="D6" s="5"/>
-      <c r="E6" s="7" t="s">
+      <c r="D6" s="9"/>
+      <c r="E6" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="F6" s="7"/>
-      <c r="G6" s="5" t="s">
+      <c r="F6" s="10"/>
+      <c r="G6" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="H6" s="5"/>
-      <c r="I6" s="5"/>
-      <c r="J6" s="5" t="s">
+      <c r="H6" s="9"/>
+      <c r="I6" s="9"/>
+      <c r="J6" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="K6" s="5"/>
-      <c r="L6" s="5"/>
-      <c r="M6" s="5" t="s">
+      <c r="K6" s="9"/>
+      <c r="L6" s="9"/>
+      <c r="M6" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="N6" s="5"/>
-      <c r="O6" s="5"/>
-      <c r="P6" s="4">
+      <c r="N6" s="9"/>
+      <c r="O6" s="9"/>
+      <c r="P6" s="12">
         <v>42707</v>
       </c>
-      <c r="Q6" s="5"/>
-      <c r="R6" s="4" t="s">
+      <c r="Q6" s="9"/>
+      <c r="R6" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="S6" s="5"/>
+      <c r="S6" s="9"/>
       <c r="T6" s="1" t="s">
         <v>38</v>
       </c>
@@ -700,37 +776,37 @@
       </c>
     </row>
     <row r="7" spans="3:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C7" s="5" t="s">
+      <c r="C7" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="D7" s="5"/>
-      <c r="E7" s="6" t="s">
+      <c r="D7" s="9"/>
+      <c r="E7" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="F7" s="6"/>
-      <c r="G7" s="5" t="s">
+      <c r="F7" s="11"/>
+      <c r="G7" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="H7" s="5"/>
-      <c r="I7" s="5"/>
-      <c r="J7" s="5" t="s">
+      <c r="H7" s="9"/>
+      <c r="I7" s="9"/>
+      <c r="J7" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="K7" s="5"/>
-      <c r="L7" s="5"/>
-      <c r="M7" s="5" t="s">
+      <c r="K7" s="9"/>
+      <c r="L7" s="9"/>
+      <c r="M7" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="N7" s="5"/>
-      <c r="O7" s="5"/>
-      <c r="P7" s="4">
+      <c r="N7" s="9"/>
+      <c r="O7" s="9"/>
+      <c r="P7" s="12">
         <v>42707</v>
       </c>
-      <c r="Q7" s="5"/>
-      <c r="R7" s="4" t="s">
+      <c r="Q7" s="9"/>
+      <c r="R7" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="S7" s="5"/>
+      <c r="S7" s="9"/>
       <c r="T7" s="1" t="s">
         <v>38</v>
       </c>
@@ -739,37 +815,37 @@
       </c>
     </row>
     <row r="8" spans="3:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C8" s="5" t="s">
+      <c r="C8" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="D8" s="5"/>
-      <c r="E8" s="6" t="s">
+      <c r="D8" s="9"/>
+      <c r="E8" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="F8" s="6"/>
-      <c r="G8" s="5" t="s">
+      <c r="F8" s="11"/>
+      <c r="G8" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="H8" s="5"/>
-      <c r="I8" s="5"/>
-      <c r="J8" s="5" t="s">
+      <c r="H8" s="9"/>
+      <c r="I8" s="9"/>
+      <c r="J8" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="K8" s="5"/>
-      <c r="L8" s="5"/>
-      <c r="M8" s="5" t="s">
+      <c r="K8" s="9"/>
+      <c r="L8" s="9"/>
+      <c r="M8" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="N8" s="5"/>
-      <c r="O8" s="5"/>
-      <c r="P8" s="4">
+      <c r="N8" s="9"/>
+      <c r="O8" s="9"/>
+      <c r="P8" s="12">
         <v>42707</v>
       </c>
-      <c r="Q8" s="5"/>
-      <c r="R8" s="4">
+      <c r="Q8" s="9"/>
+      <c r="R8" s="12">
         <v>42707</v>
       </c>
-      <c r="S8" s="5"/>
+      <c r="S8" s="9"/>
       <c r="T8" s="1" t="s">
         <v>38</v>
       </c>
@@ -778,37 +854,37 @@
       </c>
     </row>
     <row r="9" spans="3:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C9" s="5" t="s">
+      <c r="C9" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="D9" s="5"/>
-      <c r="E9" s="6" t="s">
+      <c r="D9" s="9"/>
+      <c r="E9" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="F9" s="6"/>
-      <c r="G9" s="5" t="s">
+      <c r="F9" s="11"/>
+      <c r="G9" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="H9" s="5"/>
-      <c r="I9" s="5"/>
-      <c r="J9" s="5" t="s">
+      <c r="H9" s="9"/>
+      <c r="I9" s="9"/>
+      <c r="J9" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="K9" s="5"/>
-      <c r="L9" s="5"/>
-      <c r="M9" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="N9" s="5"/>
-      <c r="O9" s="5"/>
-      <c r="P9" s="4">
+      <c r="K9" s="9"/>
+      <c r="L9" s="9"/>
+      <c r="M9" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="N9" s="9"/>
+      <c r="O9" s="9"/>
+      <c r="P9" s="12">
         <v>42707</v>
       </c>
-      <c r="Q9" s="5"/>
-      <c r="R9" s="4" t="s">
+      <c r="Q9" s="9"/>
+      <c r="R9" s="12" t="s">
         <v>35</v>
       </c>
-      <c r="S9" s="5"/>
+      <c r="S9" s="9"/>
       <c r="T9" s="1" t="s">
         <v>38</v>
       </c>
@@ -817,37 +893,37 @@
       </c>
     </row>
     <row r="10" spans="3:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C10" s="5" t="s">
+      <c r="C10" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="D10" s="5"/>
-      <c r="E10" s="7" t="s">
+      <c r="D10" s="9"/>
+      <c r="E10" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="F10" s="7"/>
-      <c r="G10" s="5" t="s">
+      <c r="F10" s="10"/>
+      <c r="G10" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="H10" s="5"/>
-      <c r="I10" s="5"/>
-      <c r="J10" s="5" t="s">
+      <c r="H10" s="9"/>
+      <c r="I10" s="9"/>
+      <c r="J10" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="K10" s="5"/>
-      <c r="L10" s="5"/>
-      <c r="M10" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="N10" s="5"/>
-      <c r="O10" s="5"/>
-      <c r="P10" s="4">
+      <c r="K10" s="9"/>
+      <c r="L10" s="9"/>
+      <c r="M10" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="N10" s="9"/>
+      <c r="O10" s="9"/>
+      <c r="P10" s="12">
         <v>42707</v>
       </c>
-      <c r="Q10" s="5"/>
-      <c r="R10" s="4" t="s">
+      <c r="Q10" s="9"/>
+      <c r="R10" s="12" t="s">
         <v>39</v>
       </c>
-      <c r="S10" s="5"/>
+      <c r="S10" s="9"/>
       <c r="T10" s="1" t="s">
         <v>38</v>
       </c>
@@ -856,37 +932,37 @@
       </c>
     </row>
     <row r="11" spans="3:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C11" s="5" t="s">
+      <c r="C11" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="D11" s="5"/>
-      <c r="E11" s="6" t="s">
+      <c r="D11" s="9"/>
+      <c r="E11" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="F11" s="6"/>
-      <c r="G11" s="5" t="s">
+      <c r="F11" s="11"/>
+      <c r="G11" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="H11" s="5"/>
-      <c r="I11" s="5"/>
-      <c r="J11" s="5" t="s">
+      <c r="H11" s="9"/>
+      <c r="I11" s="9"/>
+      <c r="J11" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="K11" s="5"/>
-      <c r="L11" s="5"/>
-      <c r="M11" s="5" t="s">
+      <c r="K11" s="9"/>
+      <c r="L11" s="9"/>
+      <c r="M11" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="N11" s="5"/>
-      <c r="O11" s="5"/>
-      <c r="P11" s="4">
+      <c r="N11" s="9"/>
+      <c r="O11" s="9"/>
+      <c r="P11" s="12">
         <v>42707</v>
       </c>
-      <c r="Q11" s="5"/>
-      <c r="R11" s="5" t="s">
+      <c r="Q11" s="9"/>
+      <c r="R11" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="S11" s="5"/>
+      <c r="S11" s="9"/>
       <c r="T11" s="1" t="s">
         <v>38</v>
       </c>
@@ -894,38 +970,38 @@
         <v>30</v>
       </c>
     </row>
-    <row r="12" spans="3:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C12" s="5" t="s">
+    <row r="12" spans="3:21" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C12" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="D12" s="5"/>
-      <c r="E12" s="7" t="s">
+      <c r="D12" s="9"/>
+      <c r="E12" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="F12" s="7"/>
-      <c r="G12" s="5" t="s">
+      <c r="F12" s="10"/>
+      <c r="G12" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="H12" s="5"/>
-      <c r="I12" s="5"/>
-      <c r="J12" s="5" t="s">
+      <c r="H12" s="9"/>
+      <c r="I12" s="9"/>
+      <c r="J12" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="K12" s="5"/>
-      <c r="L12" s="5"/>
-      <c r="M12" s="5" t="s">
+      <c r="K12" s="9"/>
+      <c r="L12" s="9"/>
+      <c r="M12" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="N12" s="5"/>
-      <c r="O12" s="5"/>
-      <c r="P12" s="4">
+      <c r="N12" s="9"/>
+      <c r="O12" s="9"/>
+      <c r="P12" s="12">
         <v>42707</v>
       </c>
-      <c r="Q12" s="5"/>
-      <c r="R12" s="5" t="s">
+      <c r="Q12" s="9"/>
+      <c r="R12" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="S12" s="5"/>
+      <c r="S12" s="9"/>
       <c r="T12" s="1" t="s">
         <v>38</v>
       </c>
@@ -933,38 +1009,38 @@
         <v>30</v>
       </c>
     </row>
-    <row r="13" spans="3:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C13" s="5" t="s">
+    <row r="13" spans="3:21" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C13" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="D13" s="5"/>
-      <c r="E13" s="5" t="s">
+      <c r="D13" s="9"/>
+      <c r="E13" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="F13" s="5"/>
-      <c r="G13" s="5" t="s">
+      <c r="F13" s="9"/>
+      <c r="G13" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="H13" s="5"/>
-      <c r="I13" s="5"/>
-      <c r="J13" s="5" t="s">
+      <c r="H13" s="9"/>
+      <c r="I13" s="9"/>
+      <c r="J13" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="K13" s="5"/>
-      <c r="L13" s="5"/>
-      <c r="M13" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="N13" s="5"/>
-      <c r="O13" s="5"/>
-      <c r="P13" s="4">
+      <c r="K13" s="9"/>
+      <c r="L13" s="9"/>
+      <c r="M13" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="N13" s="9"/>
+      <c r="O13" s="9"/>
+      <c r="P13" s="12">
         <v>42404</v>
       </c>
-      <c r="Q13" s="5"/>
-      <c r="R13" s="4">
+      <c r="Q13" s="9"/>
+      <c r="R13" s="12">
         <v>42433</v>
       </c>
-      <c r="S13" s="5"/>
+      <c r="S13" s="9"/>
       <c r="T13" s="1" t="s">
         <v>38</v>
       </c>
@@ -972,82 +1048,525 @@
         <v>30</v>
       </c>
     </row>
-    <row r="14" spans="3:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C14" s="5"/>
-      <c r="D14" s="5"/>
-      <c r="E14" s="5"/>
-      <c r="F14" s="5"/>
-      <c r="G14" s="5"/>
-      <c r="H14" s="5"/>
-      <c r="I14" s="5"/>
-      <c r="J14" s="5"/>
-      <c r="K14" s="5"/>
-      <c r="L14" s="5"/>
-      <c r="M14" s="5"/>
-      <c r="N14" s="5"/>
-      <c r="O14" s="5"/>
-      <c r="P14" s="5"/>
-      <c r="Q14" s="5"/>
-      <c r="R14" s="5"/>
-      <c r="S14" s="5"/>
-      <c r="T14" s="1"/>
-      <c r="U14" s="1"/>
-    </row>
-    <row r="15" spans="3:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C15" s="5"/>
-      <c r="D15" s="5"/>
-      <c r="E15" s="5"/>
-      <c r="F15" s="5"/>
-      <c r="G15" s="5"/>
-      <c r="H15" s="5"/>
-      <c r="I15" s="5"/>
-      <c r="J15" s="5"/>
-      <c r="K15" s="5"/>
-      <c r="L15" s="5"/>
-      <c r="M15" s="5"/>
-      <c r="N15" s="5"/>
-      <c r="O15" s="5"/>
-      <c r="P15" s="5"/>
-      <c r="Q15" s="5"/>
-      <c r="R15" s="5"/>
-      <c r="S15" s="5"/>
-      <c r="T15" s="1"/>
-      <c r="U15" s="1"/>
-    </row>
+    <row r="14" spans="3:21" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C14" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="D14" s="9"/>
+      <c r="E14" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="F14" s="9"/>
+      <c r="G14" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="H14" s="9"/>
+      <c r="I14" s="9"/>
+      <c r="J14" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="K14" s="9"/>
+      <c r="L14" s="9"/>
+      <c r="M14" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="N14" s="9"/>
+      <c r="O14" s="9"/>
+      <c r="P14" s="12">
+        <v>42404</v>
+      </c>
+      <c r="Q14" s="9"/>
+      <c r="R14" s="12">
+        <v>42434</v>
+      </c>
+      <c r="S14" s="9"/>
+      <c r="T14" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="U14" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="15" spans="3:21" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C15" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="D15" s="9"/>
+      <c r="E15" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="F15" s="9"/>
+      <c r="G15" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="H15" s="9"/>
+      <c r="I15" s="9"/>
+      <c r="J15" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="K15" s="9"/>
+      <c r="L15" s="9"/>
+      <c r="M15" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="N15" s="9"/>
+      <c r="O15" s="9"/>
+      <c r="P15" s="12">
+        <v>42406</v>
+      </c>
+      <c r="Q15" s="9"/>
+      <c r="R15" s="12">
+        <v>42435</v>
+      </c>
+      <c r="S15" s="9"/>
+      <c r="T15" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="U15" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="16" spans="3:21" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C16" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="D16" s="9"/>
+      <c r="E16" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="F16" s="9"/>
+      <c r="G16" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="H16" s="9"/>
+      <c r="I16" s="9"/>
+      <c r="J16" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="K16" s="9"/>
+      <c r="L16" s="9"/>
+      <c r="M16" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="N16" s="9"/>
+      <c r="O16" s="9"/>
+      <c r="P16" s="12">
+        <v>42407</v>
+      </c>
+      <c r="Q16" s="9"/>
+      <c r="R16" s="12">
+        <v>42436</v>
+      </c>
+      <c r="S16" s="9"/>
+      <c r="T16" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="U16" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="17" spans="3:21" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C17" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="D17" s="9"/>
+      <c r="E17" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="F17" s="9"/>
+      <c r="G17" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="H17" s="9"/>
+      <c r="I17" s="9"/>
+      <c r="J17" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="K17" s="9"/>
+      <c r="L17" s="9"/>
+      <c r="M17" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="N17" s="9"/>
+      <c r="O17" s="9"/>
+      <c r="P17" s="12">
+        <v>42407</v>
+      </c>
+      <c r="Q17" s="9"/>
+      <c r="R17" s="12">
+        <v>42436</v>
+      </c>
+      <c r="S17" s="9"/>
+      <c r="T17" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="U17" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="18" spans="3:21" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C18" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="D18" s="9"/>
+      <c r="E18" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="F18" s="9"/>
+      <c r="G18" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="H18" s="9"/>
+      <c r="I18" s="9"/>
+      <c r="J18" s="9" t="s">
+        <v>64</v>
+      </c>
+      <c r="K18" s="9"/>
+      <c r="L18" s="9"/>
+      <c r="M18" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="N18" s="9"/>
+      <c r="O18" s="9"/>
+      <c r="P18" s="12">
+        <v>42407</v>
+      </c>
+      <c r="Q18" s="9"/>
+      <c r="R18" s="12">
+        <v>42436</v>
+      </c>
+      <c r="S18" s="9"/>
+      <c r="T18" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="U18" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="19" spans="3:21" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C19" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="D19" s="9"/>
+      <c r="E19" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="F19" s="9"/>
+      <c r="G19" s="9" t="s">
+        <v>66</v>
+      </c>
+      <c r="H19" s="9"/>
+      <c r="I19" s="9"/>
+      <c r="J19" s="9" t="s">
+        <v>64</v>
+      </c>
+      <c r="K19" s="9"/>
+      <c r="L19" s="9"/>
+      <c r="M19" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="N19" s="9"/>
+      <c r="O19" s="9"/>
+      <c r="P19" s="12">
+        <v>42407</v>
+      </c>
+      <c r="Q19" s="9"/>
+      <c r="R19" s="12">
+        <v>42436</v>
+      </c>
+      <c r="S19" s="9"/>
+      <c r="T19" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="U19" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="20" spans="3:21" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C20" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="D20" s="9"/>
+      <c r="E20" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="F20" s="9"/>
+      <c r="G20" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="H20" s="9"/>
+      <c r="I20" s="9"/>
+      <c r="J20" s="9" t="s">
+        <v>64</v>
+      </c>
+      <c r="K20" s="9"/>
+      <c r="L20" s="9"/>
+      <c r="M20" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="N20" s="9"/>
+      <c r="O20" s="9"/>
+      <c r="P20" s="12">
+        <v>42407</v>
+      </c>
+      <c r="Q20" s="9"/>
+      <c r="R20" s="12">
+        <v>42436</v>
+      </c>
+      <c r="S20" s="9"/>
+      <c r="T20" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="U20" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="21" spans="3:21" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C21" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="D21" s="9"/>
+      <c r="E21" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="F21" s="9"/>
+      <c r="G21" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="H21" s="9"/>
+      <c r="I21" s="9"/>
+      <c r="J21" s="9" t="s">
+        <v>64</v>
+      </c>
+      <c r="K21" s="9"/>
+      <c r="L21" s="9"/>
+      <c r="M21" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="N21" s="9"/>
+      <c r="O21" s="9"/>
+      <c r="P21" s="12">
+        <v>42407</v>
+      </c>
+      <c r="Q21" s="9"/>
+      <c r="R21" s="12">
+        <v>42436</v>
+      </c>
+      <c r="S21" s="9"/>
+      <c r="T21" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="U21" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="22" spans="3:21" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C22" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="D22" s="9"/>
+      <c r="E22" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="F22" s="9"/>
+      <c r="G22" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="H22" s="9"/>
+      <c r="I22" s="9"/>
+      <c r="J22" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="K22" s="9"/>
+      <c r="L22" s="9"/>
+      <c r="M22" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="N22" s="9"/>
+      <c r="O22" s="9"/>
+      <c r="P22" s="12">
+        <v>42407</v>
+      </c>
+      <c r="Q22" s="9"/>
+      <c r="R22" s="12">
+        <v>42436</v>
+      </c>
+      <c r="S22" s="9"/>
+      <c r="T22" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="U22" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="23" spans="3:21" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C23" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="D23" s="9"/>
+      <c r="E23" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="F23" s="9"/>
+      <c r="G23" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="H23" s="9"/>
+      <c r="I23" s="9"/>
+      <c r="J23" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="K23" s="9"/>
+      <c r="L23" s="9"/>
+      <c r="M23" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="N23" s="9"/>
+      <c r="O23" s="9"/>
+      <c r="P23" s="12">
+        <v>42555</v>
+      </c>
+      <c r="Q23" s="9"/>
+      <c r="R23" s="12">
+        <v>42586</v>
+      </c>
+      <c r="S23" s="9"/>
+      <c r="T23" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="U23" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="24" spans="3:21" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C24" s="9"/>
+      <c r="D24" s="9"/>
+      <c r="E24" s="9"/>
+      <c r="F24" s="9"/>
+      <c r="G24" s="9"/>
+      <c r="H24" s="9"/>
+      <c r="I24" s="9"/>
+      <c r="J24" s="9"/>
+      <c r="K24" s="9"/>
+      <c r="L24" s="9"/>
+      <c r="M24" s="9"/>
+      <c r="N24" s="9"/>
+      <c r="O24" s="9"/>
+      <c r="P24" s="9"/>
+      <c r="Q24" s="9"/>
+      <c r="R24" s="9"/>
+      <c r="S24" s="9"/>
+      <c r="T24" s="1"/>
+      <c r="U24" s="1"/>
+    </row>
+    <row r="25" spans="3:21" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="J25" s="9"/>
+      <c r="K25" s="9"/>
+      <c r="L25" s="9"/>
+    </row>
+    <row r="26" spans="3:21" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="27" spans="3:21" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="28" spans="3:21" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="29" spans="3:21" customFormat="1" x14ac:dyDescent="0.3"/>
   </sheetData>
-  <mergeCells count="81">
-    <mergeCell ref="E2:F2"/>
-    <mergeCell ref="E3:F3"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="C2:D2"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="C5:D5"/>
-    <mergeCell ref="G5:I5"/>
-    <mergeCell ref="J5:L5"/>
-    <mergeCell ref="M5:O5"/>
-    <mergeCell ref="P5:Q5"/>
-    <mergeCell ref="R5:S5"/>
-    <mergeCell ref="C6:D6"/>
-    <mergeCell ref="C7:D7"/>
-    <mergeCell ref="C8:D8"/>
-    <mergeCell ref="C9:D9"/>
-    <mergeCell ref="C10:D10"/>
-    <mergeCell ref="G6:I6"/>
-    <mergeCell ref="G7:I7"/>
-    <mergeCell ref="E14:F14"/>
+  <mergeCells count="145">
+    <mergeCell ref="P20:Q20"/>
+    <mergeCell ref="R20:S20"/>
+    <mergeCell ref="C21:D21"/>
+    <mergeCell ref="E21:F21"/>
+    <mergeCell ref="G21:I21"/>
+    <mergeCell ref="J21:L21"/>
+    <mergeCell ref="M21:O21"/>
+    <mergeCell ref="P21:Q21"/>
+    <mergeCell ref="R21:S21"/>
+    <mergeCell ref="C20:D20"/>
+    <mergeCell ref="E20:F20"/>
+    <mergeCell ref="G20:I20"/>
+    <mergeCell ref="J20:L20"/>
+    <mergeCell ref="M20:O20"/>
+    <mergeCell ref="C19:D19"/>
+    <mergeCell ref="E19:F19"/>
+    <mergeCell ref="G19:I19"/>
+    <mergeCell ref="J19:L19"/>
+    <mergeCell ref="M19:O19"/>
+    <mergeCell ref="P15:Q15"/>
+    <mergeCell ref="P16:Q16"/>
+    <mergeCell ref="P23:Q23"/>
+    <mergeCell ref="M17:O17"/>
+    <mergeCell ref="P17:Q17"/>
+    <mergeCell ref="M22:O22"/>
+    <mergeCell ref="P22:Q22"/>
+    <mergeCell ref="M18:O18"/>
+    <mergeCell ref="P18:Q18"/>
+    <mergeCell ref="P19:Q19"/>
+    <mergeCell ref="M15:O15"/>
+    <mergeCell ref="M16:O16"/>
+    <mergeCell ref="M23:O23"/>
+    <mergeCell ref="J15:L15"/>
+    <mergeCell ref="J16:L16"/>
+    <mergeCell ref="J23:L23"/>
+    <mergeCell ref="J25:L25"/>
+    <mergeCell ref="G17:I17"/>
+    <mergeCell ref="G22:I22"/>
+    <mergeCell ref="J17:L17"/>
+    <mergeCell ref="J22:L22"/>
+    <mergeCell ref="G18:I18"/>
+    <mergeCell ref="J18:L18"/>
+    <mergeCell ref="P13:Q13"/>
+    <mergeCell ref="P14:Q14"/>
+    <mergeCell ref="P24:Q24"/>
+    <mergeCell ref="C15:D15"/>
+    <mergeCell ref="C16:D16"/>
+    <mergeCell ref="C23:D23"/>
     <mergeCell ref="E15:F15"/>
-    <mergeCell ref="G8:I8"/>
-    <mergeCell ref="G9:I9"/>
-    <mergeCell ref="G10:I10"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="G11:I11"/>
-    <mergeCell ref="G14:I14"/>
+    <mergeCell ref="E16:F16"/>
+    <mergeCell ref="E23:F23"/>
+    <mergeCell ref="R11:S11"/>
+    <mergeCell ref="R12:S12"/>
+    <mergeCell ref="R13:S13"/>
+    <mergeCell ref="R14:S14"/>
+    <mergeCell ref="R24:S24"/>
+    <mergeCell ref="R15:S15"/>
+    <mergeCell ref="R16:S16"/>
+    <mergeCell ref="R23:S23"/>
+    <mergeCell ref="R17:S17"/>
+    <mergeCell ref="R22:S22"/>
+    <mergeCell ref="R18:S18"/>
+    <mergeCell ref="R19:S19"/>
+    <mergeCell ref="G13:I13"/>
+    <mergeCell ref="J13:L13"/>
+    <mergeCell ref="J14:L14"/>
+    <mergeCell ref="J24:L24"/>
+    <mergeCell ref="M11:O11"/>
+    <mergeCell ref="M12:O12"/>
+    <mergeCell ref="M13:O13"/>
+    <mergeCell ref="M14:O14"/>
+    <mergeCell ref="M24:O24"/>
+    <mergeCell ref="J12:L12"/>
+    <mergeCell ref="J11:L11"/>
     <mergeCell ref="G15:I15"/>
-    <mergeCell ref="G12:I12"/>
+    <mergeCell ref="G16:I16"/>
+    <mergeCell ref="G23:I23"/>
+    <mergeCell ref="C13:D13"/>
+    <mergeCell ref="C14:D14"/>
+    <mergeCell ref="C24:D24"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="E12:F12"/>
+    <mergeCell ref="C11:D11"/>
+    <mergeCell ref="E13:F13"/>
+    <mergeCell ref="C17:D17"/>
+    <mergeCell ref="C22:D22"/>
+    <mergeCell ref="E17:F17"/>
+    <mergeCell ref="E22:F22"/>
+    <mergeCell ref="C18:D18"/>
+    <mergeCell ref="E18:F18"/>
+    <mergeCell ref="P7:Q7"/>
+    <mergeCell ref="P8:Q8"/>
+    <mergeCell ref="P9:Q9"/>
+    <mergeCell ref="P10:Q10"/>
+    <mergeCell ref="C12:D12"/>
+    <mergeCell ref="P11:Q11"/>
+    <mergeCell ref="P12:Q12"/>
     <mergeCell ref="J9:L9"/>
     <mergeCell ref="M9:O9"/>
     <mergeCell ref="J10:L10"/>
@@ -1064,39 +1583,38 @@
     <mergeCell ref="J8:L8"/>
     <mergeCell ref="M8:O8"/>
     <mergeCell ref="P6:Q6"/>
-    <mergeCell ref="P7:Q7"/>
-    <mergeCell ref="P8:Q8"/>
-    <mergeCell ref="P9:Q9"/>
-    <mergeCell ref="P10:Q10"/>
-    <mergeCell ref="C12:D12"/>
-    <mergeCell ref="C13:D13"/>
-    <mergeCell ref="C14:D14"/>
-    <mergeCell ref="C15:D15"/>
-    <mergeCell ref="E11:F11"/>
-    <mergeCell ref="E12:F12"/>
-    <mergeCell ref="C11:D11"/>
-    <mergeCell ref="E13:F13"/>
-    <mergeCell ref="G13:I13"/>
-    <mergeCell ref="J13:L13"/>
-    <mergeCell ref="J14:L14"/>
-    <mergeCell ref="J15:L15"/>
-    <mergeCell ref="M11:O11"/>
-    <mergeCell ref="M12:O12"/>
-    <mergeCell ref="M13:O13"/>
-    <mergeCell ref="M14:O14"/>
-    <mergeCell ref="M15:O15"/>
-    <mergeCell ref="J12:L12"/>
-    <mergeCell ref="J11:L11"/>
-    <mergeCell ref="R11:S11"/>
-    <mergeCell ref="R12:S12"/>
-    <mergeCell ref="R13:S13"/>
-    <mergeCell ref="R14:S14"/>
-    <mergeCell ref="R15:S15"/>
-    <mergeCell ref="P11:Q11"/>
-    <mergeCell ref="P12:Q12"/>
-    <mergeCell ref="P13:Q13"/>
-    <mergeCell ref="P14:Q14"/>
-    <mergeCell ref="P15:Q15"/>
+    <mergeCell ref="G6:I6"/>
+    <mergeCell ref="G7:I7"/>
+    <mergeCell ref="E14:F14"/>
+    <mergeCell ref="E24:F24"/>
+    <mergeCell ref="G8:I8"/>
+    <mergeCell ref="G9:I9"/>
+    <mergeCell ref="G10:I10"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="G11:I11"/>
+    <mergeCell ref="G14:I14"/>
+    <mergeCell ref="G24:I24"/>
+    <mergeCell ref="G12:I12"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="C7:D7"/>
+    <mergeCell ref="C8:D8"/>
+    <mergeCell ref="C9:D9"/>
+    <mergeCell ref="C10:D10"/>
+    <mergeCell ref="G5:I5"/>
+    <mergeCell ref="J5:L5"/>
+    <mergeCell ref="M5:O5"/>
+    <mergeCell ref="P5:Q5"/>
+    <mergeCell ref="R5:S5"/>
+    <mergeCell ref="E2:F2"/>
+    <mergeCell ref="E3:F3"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="C5:D5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Add RTM Modification (Map tags)
</commit_message>
<xml_diff>
--- a/Digital_Air_Conditional_Screen/Project Managment/Review Log Sheet/Review Log Sheet.xlsx
+++ b/Digital_Air_Conditional_Screen/Project Managment/Review Log Sheet/Review Log Sheet.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="153222"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21960" windowHeight="7728"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="12636" windowHeight="6036"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -250,7 +250,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -271,18 +271,24 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFF0000"/>
+        <fgColor theme="7" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="-0.249977111117893"/>
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="-0.249977111117893"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -340,22 +346,39 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="14" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -364,17 +387,23 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -656,10 +685,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C1:U29"/>
+  <dimension ref="C1:U30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J25" sqref="J25:L25"/>
+    <sheetView tabSelected="1" topLeftCell="K8" workbookViewId="0">
+      <selection activeCell="R24" sqref="R24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -672,24 +701,24 @@
   <sheetData>
     <row r="1" spans="3:21" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="3:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C2" s="7" t="s">
+      <c r="C2" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="8"/>
-      <c r="E2" s="4" t="s">
+      <c r="D2" s="10"/>
+      <c r="E2" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="F2" s="5"/>
+      <c r="F2" s="8"/>
     </row>
     <row r="3" spans="3:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C3" s="7" t="s">
+      <c r="C3" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="8"/>
-      <c r="E3" s="4" t="s">
+      <c r="D3" s="10"/>
+      <c r="E3" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="F3" s="5"/>
+      <c r="F3" s="8"/>
     </row>
     <row r="4" spans="3:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C4" s="2"/>
@@ -737,37 +766,37 @@
       </c>
     </row>
     <row r="6" spans="3:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C6" s="9" t="s">
+      <c r="C6" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="D6" s="9"/>
-      <c r="E6" s="10" t="s">
+      <c r="D6" s="5"/>
+      <c r="E6" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="F6" s="10"/>
-      <c r="G6" s="9" t="s">
+      <c r="F6" s="13"/>
+      <c r="G6" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="H6" s="9"/>
-      <c r="I6" s="9"/>
-      <c r="J6" s="9" t="s">
+      <c r="H6" s="5"/>
+      <c r="I6" s="5"/>
+      <c r="J6" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="K6" s="9"/>
-      <c r="L6" s="9"/>
-      <c r="M6" s="9" t="s">
+      <c r="K6" s="5"/>
+      <c r="L6" s="5"/>
+      <c r="M6" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="N6" s="9"/>
-      <c r="O6" s="9"/>
-      <c r="P6" s="12">
+      <c r="N6" s="5"/>
+      <c r="O6" s="5"/>
+      <c r="P6" s="4">
         <v>42707</v>
       </c>
-      <c r="Q6" s="9"/>
-      <c r="R6" s="12" t="s">
+      <c r="Q6" s="5"/>
+      <c r="R6" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="S6" s="9"/>
+      <c r="S6" s="5"/>
       <c r="T6" s="1" t="s">
         <v>38</v>
       </c>
@@ -776,37 +805,37 @@
       </c>
     </row>
     <row r="7" spans="3:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C7" s="9" t="s">
+      <c r="C7" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="D7" s="9"/>
+      <c r="D7" s="5"/>
       <c r="E7" s="11" t="s">
         <v>24</v>
       </c>
       <c r="F7" s="11"/>
-      <c r="G7" s="9" t="s">
+      <c r="G7" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="H7" s="9"/>
-      <c r="I7" s="9"/>
-      <c r="J7" s="9" t="s">
+      <c r="H7" s="5"/>
+      <c r="I7" s="5"/>
+      <c r="J7" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="K7" s="9"/>
-      <c r="L7" s="9"/>
-      <c r="M7" s="9" t="s">
+      <c r="K7" s="5"/>
+      <c r="L7" s="5"/>
+      <c r="M7" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="N7" s="9"/>
-      <c r="O7" s="9"/>
-      <c r="P7" s="12">
+      <c r="N7" s="5"/>
+      <c r="O7" s="5"/>
+      <c r="P7" s="4">
         <v>42707</v>
       </c>
-      <c r="Q7" s="9"/>
-      <c r="R7" s="12" t="s">
+      <c r="Q7" s="5"/>
+      <c r="R7" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="S7" s="9"/>
+      <c r="S7" s="5"/>
       <c r="T7" s="1" t="s">
         <v>38</v>
       </c>
@@ -815,37 +844,37 @@
       </c>
     </row>
     <row r="8" spans="3:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C8" s="9" t="s">
+      <c r="C8" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="D8" s="9"/>
+      <c r="D8" s="5"/>
       <c r="E8" s="11" t="s">
         <v>24</v>
       </c>
       <c r="F8" s="11"/>
-      <c r="G8" s="9" t="s">
+      <c r="G8" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="H8" s="9"/>
-      <c r="I8" s="9"/>
-      <c r="J8" s="9" t="s">
+      <c r="H8" s="5"/>
+      <c r="I8" s="5"/>
+      <c r="J8" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="K8" s="9"/>
-      <c r="L8" s="9"/>
-      <c r="M8" s="9" t="s">
+      <c r="K8" s="5"/>
+      <c r="L8" s="5"/>
+      <c r="M8" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="N8" s="9"/>
-      <c r="O8" s="9"/>
-      <c r="P8" s="12">
+      <c r="N8" s="5"/>
+      <c r="O8" s="5"/>
+      <c r="P8" s="4">
         <v>42707</v>
       </c>
-      <c r="Q8" s="9"/>
-      <c r="R8" s="12">
+      <c r="Q8" s="5"/>
+      <c r="R8" s="4">
         <v>42707</v>
       </c>
-      <c r="S8" s="9"/>
+      <c r="S8" s="5"/>
       <c r="T8" s="1" t="s">
         <v>38</v>
       </c>
@@ -854,37 +883,37 @@
       </c>
     </row>
     <row r="9" spans="3:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C9" s="9" t="s">
+      <c r="C9" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="D9" s="9"/>
+      <c r="D9" s="5"/>
       <c r="E9" s="11" t="s">
         <v>24</v>
       </c>
       <c r="F9" s="11"/>
-      <c r="G9" s="9" t="s">
+      <c r="G9" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="H9" s="9"/>
-      <c r="I9" s="9"/>
-      <c r="J9" s="9" t="s">
+      <c r="H9" s="5"/>
+      <c r="I9" s="5"/>
+      <c r="J9" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="K9" s="9"/>
-      <c r="L9" s="9"/>
-      <c r="M9" s="9" t="s">
-        <v>30</v>
-      </c>
-      <c r="N9" s="9"/>
-      <c r="O9" s="9"/>
-      <c r="P9" s="12">
+      <c r="K9" s="5"/>
+      <c r="L9" s="5"/>
+      <c r="M9" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="N9" s="5"/>
+      <c r="O9" s="5"/>
+      <c r="P9" s="4">
         <v>42707</v>
       </c>
-      <c r="Q9" s="9"/>
-      <c r="R9" s="12" t="s">
+      <c r="Q9" s="5"/>
+      <c r="R9" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="S9" s="9"/>
+      <c r="S9" s="5"/>
       <c r="T9" s="1" t="s">
         <v>38</v>
       </c>
@@ -893,37 +922,37 @@
       </c>
     </row>
     <row r="10" spans="3:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C10" s="9" t="s">
+      <c r="C10" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="D10" s="9"/>
-      <c r="E10" s="10" t="s">
+      <c r="D10" s="5"/>
+      <c r="E10" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="F10" s="10"/>
-      <c r="G10" s="9" t="s">
+      <c r="F10" s="13"/>
+      <c r="G10" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="H10" s="9"/>
-      <c r="I10" s="9"/>
-      <c r="J10" s="9" t="s">
+      <c r="H10" s="5"/>
+      <c r="I10" s="5"/>
+      <c r="J10" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="K10" s="9"/>
-      <c r="L10" s="9"/>
-      <c r="M10" s="9" t="s">
-        <v>30</v>
-      </c>
-      <c r="N10" s="9"/>
-      <c r="O10" s="9"/>
-      <c r="P10" s="12">
+      <c r="K10" s="5"/>
+      <c r="L10" s="5"/>
+      <c r="M10" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="N10" s="5"/>
+      <c r="O10" s="5"/>
+      <c r="P10" s="4">
         <v>42707</v>
       </c>
-      <c r="Q10" s="9"/>
-      <c r="R10" s="12" t="s">
+      <c r="Q10" s="5"/>
+      <c r="R10" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="S10" s="9"/>
+      <c r="S10" s="5"/>
       <c r="T10" s="1" t="s">
         <v>38</v>
       </c>
@@ -932,37 +961,37 @@
       </c>
     </row>
     <row r="11" spans="3:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C11" s="9" t="s">
+      <c r="C11" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="D11" s="9"/>
+      <c r="D11" s="5"/>
       <c r="E11" s="11" t="s">
         <v>24</v>
       </c>
       <c r="F11" s="11"/>
-      <c r="G11" s="9" t="s">
+      <c r="G11" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="H11" s="9"/>
-      <c r="I11" s="9"/>
-      <c r="J11" s="9" t="s">
+      <c r="H11" s="5"/>
+      <c r="I11" s="5"/>
+      <c r="J11" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="K11" s="9"/>
-      <c r="L11" s="9"/>
-      <c r="M11" s="9" t="s">
+      <c r="K11" s="5"/>
+      <c r="L11" s="5"/>
+      <c r="M11" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="N11" s="9"/>
-      <c r="O11" s="9"/>
-      <c r="P11" s="12">
+      <c r="N11" s="5"/>
+      <c r="O11" s="5"/>
+      <c r="P11" s="4">
         <v>42707</v>
       </c>
-      <c r="Q11" s="9"/>
-      <c r="R11" s="9" t="s">
+      <c r="Q11" s="5"/>
+      <c r="R11" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="S11" s="9"/>
+      <c r="S11" s="5"/>
       <c r="T11" s="1" t="s">
         <v>38</v>
       </c>
@@ -971,37 +1000,37 @@
       </c>
     </row>
     <row r="12" spans="3:21" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C12" s="9" t="s">
+      <c r="C12" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="D12" s="9"/>
-      <c r="E12" s="10" t="s">
+      <c r="D12" s="5"/>
+      <c r="E12" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="F12" s="10"/>
-      <c r="G12" s="9" t="s">
+      <c r="F12" s="13"/>
+      <c r="G12" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="H12" s="9"/>
-      <c r="I12" s="9"/>
-      <c r="J12" s="9" t="s">
+      <c r="H12" s="5"/>
+      <c r="I12" s="5"/>
+      <c r="J12" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="K12" s="9"/>
-      <c r="L12" s="9"/>
-      <c r="M12" s="9" t="s">
+      <c r="K12" s="5"/>
+      <c r="L12" s="5"/>
+      <c r="M12" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="N12" s="9"/>
-      <c r="O12" s="9"/>
-      <c r="P12" s="12">
+      <c r="N12" s="5"/>
+      <c r="O12" s="5"/>
+      <c r="P12" s="4">
         <v>42707</v>
       </c>
-      <c r="Q12" s="9"/>
-      <c r="R12" s="9" t="s">
+      <c r="Q12" s="5"/>
+      <c r="R12" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="S12" s="9"/>
+      <c r="S12" s="5"/>
       <c r="T12" s="1" t="s">
         <v>38</v>
       </c>
@@ -1010,37 +1039,37 @@
       </c>
     </row>
     <row r="13" spans="3:21" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C13" s="9" t="s">
+      <c r="C13" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="D13" s="9"/>
-      <c r="E13" s="9" t="s">
+      <c r="D13" s="5"/>
+      <c r="E13" s="12" t="s">
         <v>41</v>
       </c>
-      <c r="F13" s="9"/>
-      <c r="G13" s="9" t="s">
+      <c r="F13" s="12"/>
+      <c r="G13" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="H13" s="9"/>
-      <c r="I13" s="9"/>
-      <c r="J13" s="9" t="s">
+      <c r="H13" s="5"/>
+      <c r="I13" s="5"/>
+      <c r="J13" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="K13" s="9"/>
-      <c r="L13" s="9"/>
-      <c r="M13" s="9" t="s">
-        <v>30</v>
-      </c>
-      <c r="N13" s="9"/>
-      <c r="O13" s="9"/>
-      <c r="P13" s="12">
+      <c r="K13" s="5"/>
+      <c r="L13" s="5"/>
+      <c r="M13" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="N13" s="5"/>
+      <c r="O13" s="5"/>
+      <c r="P13" s="4">
         <v>42404</v>
       </c>
-      <c r="Q13" s="9"/>
-      <c r="R13" s="12">
+      <c r="Q13" s="5"/>
+      <c r="R13" s="4">
         <v>42433</v>
       </c>
-      <c r="S13" s="9"/>
+      <c r="S13" s="5"/>
       <c r="T13" s="1" t="s">
         <v>38</v>
       </c>
@@ -1049,37 +1078,37 @@
       </c>
     </row>
     <row r="14" spans="3:21" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C14" s="9" t="s">
+      <c r="C14" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="D14" s="9"/>
-      <c r="E14" s="9" t="s">
+      <c r="D14" s="5"/>
+      <c r="E14" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="F14" s="9"/>
-      <c r="G14" s="9" t="s">
+      <c r="F14" s="13"/>
+      <c r="G14" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="H14" s="9"/>
-      <c r="I14" s="9"/>
-      <c r="J14" s="9" t="s">
+      <c r="H14" s="5"/>
+      <c r="I14" s="5"/>
+      <c r="J14" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="K14" s="9"/>
-      <c r="L14" s="9"/>
-      <c r="M14" s="9" t="s">
+      <c r="K14" s="5"/>
+      <c r="L14" s="5"/>
+      <c r="M14" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="N14" s="9"/>
-      <c r="O14" s="9"/>
-      <c r="P14" s="12">
+      <c r="N14" s="5"/>
+      <c r="O14" s="5"/>
+      <c r="P14" s="4">
         <v>42404</v>
       </c>
-      <c r="Q14" s="9"/>
-      <c r="R14" s="12">
-        <v>42434</v>
-      </c>
-      <c r="S14" s="9"/>
+      <c r="Q14" s="5"/>
+      <c r="R14" s="4">
+        <v>42433</v>
+      </c>
+      <c r="S14" s="5"/>
       <c r="T14" s="1" t="s">
         <v>38</v>
       </c>
@@ -1088,37 +1117,37 @@
       </c>
     </row>
     <row r="15" spans="3:21" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C15" s="9" t="s">
+      <c r="C15" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="D15" s="9"/>
-      <c r="E15" s="9" t="s">
+      <c r="D15" s="5"/>
+      <c r="E15" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="F15" s="9"/>
-      <c r="G15" s="9" t="s">
+      <c r="F15" s="13"/>
+      <c r="G15" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="H15" s="9"/>
-      <c r="I15" s="9"/>
-      <c r="J15" s="9" t="s">
+      <c r="H15" s="5"/>
+      <c r="I15" s="5"/>
+      <c r="J15" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="K15" s="9"/>
-      <c r="L15" s="9"/>
-      <c r="M15" s="9" t="s">
+      <c r="K15" s="5"/>
+      <c r="L15" s="5"/>
+      <c r="M15" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="N15" s="9"/>
-      <c r="O15" s="9"/>
-      <c r="P15" s="12">
-        <v>42406</v>
-      </c>
-      <c r="Q15" s="9"/>
-      <c r="R15" s="12">
-        <v>42435</v>
-      </c>
-      <c r="S15" s="9"/>
+      <c r="N15" s="5"/>
+      <c r="O15" s="5"/>
+      <c r="P15" s="4">
+        <v>42433</v>
+      </c>
+      <c r="Q15" s="5"/>
+      <c r="R15" s="4">
+        <v>42464</v>
+      </c>
+      <c r="S15" s="5"/>
       <c r="T15" s="1" t="s">
         <v>38</v>
       </c>
@@ -1127,37 +1156,37 @@
       </c>
     </row>
     <row r="16" spans="3:21" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C16" s="9" t="s">
+      <c r="C16" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="D16" s="9"/>
-      <c r="E16" s="9" t="s">
+      <c r="D16" s="5"/>
+      <c r="E16" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="F16" s="9"/>
-      <c r="G16" s="9" t="s">
+      <c r="F16" s="11"/>
+      <c r="G16" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="H16" s="9"/>
-      <c r="I16" s="9"/>
-      <c r="J16" s="9" t="s">
+      <c r="H16" s="5"/>
+      <c r="I16" s="5"/>
+      <c r="J16" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="K16" s="9"/>
-      <c r="L16" s="9"/>
-      <c r="M16" s="9" t="s">
+      <c r="K16" s="5"/>
+      <c r="L16" s="5"/>
+      <c r="M16" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="N16" s="9"/>
-      <c r="O16" s="9"/>
-      <c r="P16" s="12">
-        <v>42407</v>
-      </c>
-      <c r="Q16" s="9"/>
-      <c r="R16" s="12">
-        <v>42436</v>
-      </c>
-      <c r="S16" s="9"/>
+      <c r="N16" s="5"/>
+      <c r="O16" s="5"/>
+      <c r="P16" s="4">
+        <v>42433</v>
+      </c>
+      <c r="Q16" s="5"/>
+      <c r="R16" s="4">
+        <v>42464</v>
+      </c>
+      <c r="S16" s="5"/>
       <c r="T16" s="1" t="s">
         <v>38</v>
       </c>
@@ -1166,37 +1195,37 @@
       </c>
     </row>
     <row r="17" spans="3:21" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C17" s="9" t="s">
+      <c r="C17" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="D17" s="9"/>
-      <c r="E17" s="9" t="s">
+      <c r="D17" s="5"/>
+      <c r="E17" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="F17" s="9"/>
-      <c r="G17" s="9" t="s">
+      <c r="F17" s="11"/>
+      <c r="G17" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="H17" s="9"/>
-      <c r="I17" s="9"/>
-      <c r="J17" s="9" t="s">
+      <c r="H17" s="5"/>
+      <c r="I17" s="5"/>
+      <c r="J17" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="K17" s="9"/>
-      <c r="L17" s="9"/>
-      <c r="M17" s="9" t="s">
+      <c r="K17" s="5"/>
+      <c r="L17" s="5"/>
+      <c r="M17" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="N17" s="9"/>
-      <c r="O17" s="9"/>
-      <c r="P17" s="12">
-        <v>42407</v>
-      </c>
-      <c r="Q17" s="9"/>
-      <c r="R17" s="12">
-        <v>42436</v>
-      </c>
-      <c r="S17" s="9"/>
+      <c r="N17" s="5"/>
+      <c r="O17" s="5"/>
+      <c r="P17" s="4">
+        <v>42494</v>
+      </c>
+      <c r="Q17" s="5"/>
+      <c r="R17" s="4">
+        <v>42525</v>
+      </c>
+      <c r="S17" s="5"/>
       <c r="T17" s="1" t="s">
         <v>38</v>
       </c>
@@ -1205,37 +1234,37 @@
       </c>
     </row>
     <row r="18" spans="3:21" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C18" s="9" t="s">
+      <c r="C18" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="D18" s="9"/>
-      <c r="E18" s="9" t="s">
+      <c r="D18" s="5"/>
+      <c r="E18" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="F18" s="9"/>
-      <c r="G18" s="9" t="s">
+      <c r="F18" s="11"/>
+      <c r="G18" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="H18" s="9"/>
-      <c r="I18" s="9"/>
-      <c r="J18" s="9" t="s">
+      <c r="H18" s="5"/>
+      <c r="I18" s="5"/>
+      <c r="J18" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="K18" s="9"/>
-      <c r="L18" s="9"/>
-      <c r="M18" s="9" t="s">
+      <c r="K18" s="5"/>
+      <c r="L18" s="5"/>
+      <c r="M18" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="N18" s="9"/>
-      <c r="O18" s="9"/>
-      <c r="P18" s="12">
-        <v>42407</v>
-      </c>
-      <c r="Q18" s="9"/>
-      <c r="R18" s="12">
-        <v>42436</v>
-      </c>
-      <c r="S18" s="9"/>
+      <c r="N18" s="5"/>
+      <c r="O18" s="5"/>
+      <c r="P18" s="4">
+        <v>42525</v>
+      </c>
+      <c r="Q18" s="5"/>
+      <c r="R18" s="4">
+        <v>42555</v>
+      </c>
+      <c r="S18" s="5"/>
       <c r="T18" s="1" t="s">
         <v>38</v>
       </c>
@@ -1244,37 +1273,37 @@
       </c>
     </row>
     <row r="19" spans="3:21" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C19" s="9" t="s">
+      <c r="C19" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="D19" s="9"/>
-      <c r="E19" s="9" t="s">
+      <c r="D19" s="5"/>
+      <c r="E19" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="F19" s="9"/>
-      <c r="G19" s="9" t="s">
+      <c r="F19" s="11"/>
+      <c r="G19" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="H19" s="9"/>
-      <c r="I19" s="9"/>
-      <c r="J19" s="9" t="s">
+      <c r="H19" s="5"/>
+      <c r="I19" s="5"/>
+      <c r="J19" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="K19" s="9"/>
-      <c r="L19" s="9"/>
-      <c r="M19" s="9" t="s">
+      <c r="K19" s="5"/>
+      <c r="L19" s="5"/>
+      <c r="M19" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="N19" s="9"/>
-      <c r="O19" s="9"/>
-      <c r="P19" s="12">
-        <v>42407</v>
-      </c>
-      <c r="Q19" s="9"/>
-      <c r="R19" s="12">
-        <v>42436</v>
-      </c>
-      <c r="S19" s="9"/>
+      <c r="N19" s="5"/>
+      <c r="O19" s="5"/>
+      <c r="P19" s="4">
+        <v>42525</v>
+      </c>
+      <c r="Q19" s="5"/>
+      <c r="R19" s="4">
+        <v>42555</v>
+      </c>
+      <c r="S19" s="5"/>
       <c r="T19" s="1" t="s">
         <v>38</v>
       </c>
@@ -1283,37 +1312,37 @@
       </c>
     </row>
     <row r="20" spans="3:21" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C20" s="9" t="s">
+      <c r="C20" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="D20" s="9"/>
-      <c r="E20" s="9" t="s">
+      <c r="D20" s="5"/>
+      <c r="E20" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="F20" s="9"/>
-      <c r="G20" s="9" t="s">
+      <c r="F20" s="11"/>
+      <c r="G20" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="H20" s="9"/>
-      <c r="I20" s="9"/>
-      <c r="J20" s="9" t="s">
+      <c r="H20" s="5"/>
+      <c r="I20" s="5"/>
+      <c r="J20" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="K20" s="9"/>
-      <c r="L20" s="9"/>
-      <c r="M20" s="9" t="s">
+      <c r="K20" s="5"/>
+      <c r="L20" s="5"/>
+      <c r="M20" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="N20" s="9"/>
-      <c r="O20" s="9"/>
-      <c r="P20" s="12">
-        <v>42407</v>
-      </c>
-      <c r="Q20" s="9"/>
-      <c r="R20" s="12">
-        <v>42436</v>
-      </c>
-      <c r="S20" s="9"/>
+      <c r="N20" s="5"/>
+      <c r="O20" s="5"/>
+      <c r="P20" s="4">
+        <v>42525</v>
+      </c>
+      <c r="Q20" s="5"/>
+      <c r="R20" s="4">
+        <v>42555</v>
+      </c>
+      <c r="S20" s="5"/>
       <c r="T20" s="1" t="s">
         <v>38</v>
       </c>
@@ -1322,37 +1351,37 @@
       </c>
     </row>
     <row r="21" spans="3:21" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C21" s="9" t="s">
+      <c r="C21" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="D21" s="9"/>
-      <c r="E21" s="9" t="s">
+      <c r="D21" s="5"/>
+      <c r="E21" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="F21" s="9"/>
-      <c r="G21" s="9" t="s">
+      <c r="F21" s="11"/>
+      <c r="G21" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="H21" s="9"/>
-      <c r="I21" s="9"/>
-      <c r="J21" s="9" t="s">
+      <c r="H21" s="5"/>
+      <c r="I21" s="5"/>
+      <c r="J21" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="K21" s="9"/>
-      <c r="L21" s="9"/>
-      <c r="M21" s="9" t="s">
+      <c r="K21" s="5"/>
+      <c r="L21" s="5"/>
+      <c r="M21" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="N21" s="9"/>
-      <c r="O21" s="9"/>
-      <c r="P21" s="12">
-        <v>42407</v>
-      </c>
-      <c r="Q21" s="9"/>
-      <c r="R21" s="12">
-        <v>42436</v>
-      </c>
-      <c r="S21" s="9"/>
+      <c r="N21" s="5"/>
+      <c r="O21" s="5"/>
+      <c r="P21" s="4">
+        <v>42525</v>
+      </c>
+      <c r="Q21" s="5"/>
+      <c r="R21" s="4">
+        <v>42555</v>
+      </c>
+      <c r="S21" s="5"/>
       <c r="T21" s="1" t="s">
         <v>38</v>
       </c>
@@ -1361,37 +1390,37 @@
       </c>
     </row>
     <row r="22" spans="3:21" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C22" s="9" t="s">
+      <c r="C22" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="D22" s="9"/>
-      <c r="E22" s="9" t="s">
+      <c r="D22" s="5"/>
+      <c r="E22" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="F22" s="9"/>
-      <c r="G22" s="9" t="s">
+      <c r="F22" s="11"/>
+      <c r="G22" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="H22" s="9"/>
-      <c r="I22" s="9"/>
-      <c r="J22" s="9" t="s">
+      <c r="H22" s="5"/>
+      <c r="I22" s="5"/>
+      <c r="J22" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="K22" s="9"/>
-      <c r="L22" s="9"/>
-      <c r="M22" s="9" t="s">
+      <c r="K22" s="5"/>
+      <c r="L22" s="5"/>
+      <c r="M22" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="N22" s="9"/>
-      <c r="O22" s="9"/>
-      <c r="P22" s="12">
-        <v>42407</v>
-      </c>
-      <c r="Q22" s="9"/>
-      <c r="R22" s="12">
-        <v>42436</v>
-      </c>
-      <c r="S22" s="9"/>
+      <c r="N22" s="5"/>
+      <c r="O22" s="5"/>
+      <c r="P22" s="4">
+        <v>42525</v>
+      </c>
+      <c r="Q22" s="5"/>
+      <c r="R22" s="4">
+        <v>42555</v>
+      </c>
+      <c r="S22" s="5"/>
       <c r="T22" s="1" t="s">
         <v>38</v>
       </c>
@@ -1400,37 +1429,37 @@
       </c>
     </row>
     <row r="23" spans="3:21" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C23" s="9" t="s">
+      <c r="C23" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="D23" s="9"/>
-      <c r="E23" s="9" t="s">
+      <c r="D23" s="5"/>
+      <c r="E23" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="F23" s="9"/>
-      <c r="G23" s="9" t="s">
+      <c r="F23" s="13"/>
+      <c r="G23" s="14" t="s">
         <v>50</v>
       </c>
-      <c r="H23" s="9"/>
-      <c r="I23" s="9"/>
-      <c r="J23" s="9" t="s">
+      <c r="H23" s="15"/>
+      <c r="I23" s="16"/>
+      <c r="J23" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="K23" s="9"/>
-      <c r="L23" s="9"/>
-      <c r="M23" s="9" t="s">
+      <c r="K23" s="5"/>
+      <c r="L23" s="5"/>
+      <c r="M23" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="N23" s="9"/>
-      <c r="O23" s="9"/>
-      <c r="P23" s="12">
+      <c r="N23" s="5"/>
+      <c r="O23" s="5"/>
+      <c r="P23" s="4">
         <v>42555</v>
       </c>
-      <c r="Q23" s="9"/>
-      <c r="R23" s="12">
+      <c r="Q23" s="5"/>
+      <c r="R23" s="4">
         <v>42586</v>
       </c>
-      <c r="S23" s="9"/>
+      <c r="S23" s="5"/>
       <c r="T23" s="1" t="s">
         <v>38</v>
       </c>
@@ -1438,38 +1467,138 @@
         <v>30</v>
       </c>
     </row>
-    <row r="24" spans="3:21" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C24" s="9"/>
-      <c r="D24" s="9"/>
-      <c r="E24" s="9"/>
-      <c r="F24" s="9"/>
-      <c r="G24" s="9"/>
-      <c r="H24" s="9"/>
-      <c r="I24" s="9"/>
-      <c r="J24" s="9"/>
-      <c r="K24" s="9"/>
-      <c r="L24" s="9"/>
-      <c r="M24" s="9"/>
-      <c r="N24" s="9"/>
-      <c r="O24" s="9"/>
-      <c r="P24" s="9"/>
-      <c r="Q24" s="9"/>
-      <c r="R24" s="9"/>
-      <c r="S24" s="9"/>
-      <c r="T24" s="1"/>
-      <c r="U24" s="1"/>
-    </row>
-    <row r="25" spans="3:21" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="J25" s="9"/>
-      <c r="K25" s="9"/>
-      <c r="L25" s="9"/>
-    </row>
+    <row r="24" spans="3:21" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="25" spans="3:21" customFormat="1" x14ac:dyDescent="0.3"/>
     <row r="26" spans="3:21" customFormat="1" x14ac:dyDescent="0.3"/>
     <row r="27" spans="3:21" customFormat="1" x14ac:dyDescent="0.3"/>
     <row r="28" spans="3:21" customFormat="1" x14ac:dyDescent="0.3"/>
     <row r="29" spans="3:21" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="30" spans="3:21" customFormat="1" x14ac:dyDescent="0.3"/>
   </sheetData>
-  <mergeCells count="145">
+  <mergeCells count="137">
+    <mergeCell ref="R5:S5"/>
+    <mergeCell ref="E2:F2"/>
+    <mergeCell ref="E3:F3"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="C23:D23"/>
+    <mergeCell ref="E23:F23"/>
+    <mergeCell ref="J23:L23"/>
+    <mergeCell ref="M23:O23"/>
+    <mergeCell ref="P23:Q23"/>
+    <mergeCell ref="R23:S23"/>
+    <mergeCell ref="G23:I23"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="C7:D7"/>
+    <mergeCell ref="C8:D8"/>
+    <mergeCell ref="C9:D9"/>
+    <mergeCell ref="C10:D10"/>
+    <mergeCell ref="G5:I5"/>
+    <mergeCell ref="J5:L5"/>
+    <mergeCell ref="M5:O5"/>
+    <mergeCell ref="P5:Q5"/>
+    <mergeCell ref="G6:I6"/>
+    <mergeCell ref="G7:I7"/>
+    <mergeCell ref="E14:F14"/>
+    <mergeCell ref="G8:I8"/>
+    <mergeCell ref="G9:I9"/>
+    <mergeCell ref="G10:I10"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="G11:I11"/>
+    <mergeCell ref="G14:I14"/>
+    <mergeCell ref="G12:I12"/>
+    <mergeCell ref="R6:S6"/>
+    <mergeCell ref="R7:S7"/>
+    <mergeCell ref="R8:S8"/>
+    <mergeCell ref="R9:S9"/>
+    <mergeCell ref="R10:S10"/>
+    <mergeCell ref="J6:L6"/>
+    <mergeCell ref="M6:O6"/>
+    <mergeCell ref="J7:L7"/>
+    <mergeCell ref="M7:O7"/>
+    <mergeCell ref="J8:L8"/>
+    <mergeCell ref="M8:O8"/>
+    <mergeCell ref="P6:Q6"/>
+    <mergeCell ref="P7:Q7"/>
+    <mergeCell ref="P8:Q8"/>
+    <mergeCell ref="P9:Q9"/>
+    <mergeCell ref="P10:Q10"/>
+    <mergeCell ref="C12:D12"/>
+    <mergeCell ref="P11:Q11"/>
+    <mergeCell ref="P12:Q12"/>
+    <mergeCell ref="J9:L9"/>
+    <mergeCell ref="M9:O9"/>
+    <mergeCell ref="J10:L10"/>
+    <mergeCell ref="M10:O10"/>
+    <mergeCell ref="J12:L12"/>
+    <mergeCell ref="J11:L11"/>
+    <mergeCell ref="G15:I15"/>
+    <mergeCell ref="G16:I16"/>
+    <mergeCell ref="C13:D13"/>
+    <mergeCell ref="C14:D14"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="E12:F12"/>
+    <mergeCell ref="C11:D11"/>
+    <mergeCell ref="E13:F13"/>
+    <mergeCell ref="C17:D17"/>
+    <mergeCell ref="C22:D22"/>
+    <mergeCell ref="E17:F17"/>
+    <mergeCell ref="E22:F22"/>
+    <mergeCell ref="C18:D18"/>
+    <mergeCell ref="E18:F18"/>
+    <mergeCell ref="E15:F15"/>
+    <mergeCell ref="E16:F16"/>
+    <mergeCell ref="R11:S11"/>
+    <mergeCell ref="R12:S12"/>
+    <mergeCell ref="R13:S13"/>
+    <mergeCell ref="R14:S14"/>
+    <mergeCell ref="R15:S15"/>
+    <mergeCell ref="R16:S16"/>
+    <mergeCell ref="R17:S17"/>
+    <mergeCell ref="R22:S22"/>
+    <mergeCell ref="R18:S18"/>
+    <mergeCell ref="R19:S19"/>
+    <mergeCell ref="G13:I13"/>
+    <mergeCell ref="J13:L13"/>
+    <mergeCell ref="J14:L14"/>
+    <mergeCell ref="M11:O11"/>
+    <mergeCell ref="M12:O12"/>
+    <mergeCell ref="M13:O13"/>
+    <mergeCell ref="M14:O14"/>
+    <mergeCell ref="G17:I17"/>
+    <mergeCell ref="G22:I22"/>
+    <mergeCell ref="J17:L17"/>
+    <mergeCell ref="J22:L22"/>
+    <mergeCell ref="G18:I18"/>
+    <mergeCell ref="J18:L18"/>
+    <mergeCell ref="P13:Q13"/>
+    <mergeCell ref="P14:Q14"/>
+    <mergeCell ref="C19:D19"/>
+    <mergeCell ref="E19:F19"/>
+    <mergeCell ref="G19:I19"/>
+    <mergeCell ref="J19:L19"/>
+    <mergeCell ref="M19:O19"/>
+    <mergeCell ref="P15:Q15"/>
+    <mergeCell ref="P16:Q16"/>
+    <mergeCell ref="M17:O17"/>
+    <mergeCell ref="P17:Q17"/>
+    <mergeCell ref="M22:O22"/>
+    <mergeCell ref="P22:Q22"/>
+    <mergeCell ref="M18:O18"/>
+    <mergeCell ref="P18:Q18"/>
+    <mergeCell ref="P19:Q19"/>
+    <mergeCell ref="M15:O15"/>
+    <mergeCell ref="M16:O16"/>
+    <mergeCell ref="J15:L15"/>
+    <mergeCell ref="J16:L16"/>
+    <mergeCell ref="C15:D15"/>
+    <mergeCell ref="C16:D16"/>
     <mergeCell ref="P20:Q20"/>
     <mergeCell ref="R20:S20"/>
     <mergeCell ref="C21:D21"/>
@@ -1484,137 +1613,6 @@
     <mergeCell ref="G20:I20"/>
     <mergeCell ref="J20:L20"/>
     <mergeCell ref="M20:O20"/>
-    <mergeCell ref="C19:D19"/>
-    <mergeCell ref="E19:F19"/>
-    <mergeCell ref="G19:I19"/>
-    <mergeCell ref="J19:L19"/>
-    <mergeCell ref="M19:O19"/>
-    <mergeCell ref="P15:Q15"/>
-    <mergeCell ref="P16:Q16"/>
-    <mergeCell ref="P23:Q23"/>
-    <mergeCell ref="M17:O17"/>
-    <mergeCell ref="P17:Q17"/>
-    <mergeCell ref="M22:O22"/>
-    <mergeCell ref="P22:Q22"/>
-    <mergeCell ref="M18:O18"/>
-    <mergeCell ref="P18:Q18"/>
-    <mergeCell ref="P19:Q19"/>
-    <mergeCell ref="M15:O15"/>
-    <mergeCell ref="M16:O16"/>
-    <mergeCell ref="M23:O23"/>
-    <mergeCell ref="J15:L15"/>
-    <mergeCell ref="J16:L16"/>
-    <mergeCell ref="J23:L23"/>
-    <mergeCell ref="J25:L25"/>
-    <mergeCell ref="G17:I17"/>
-    <mergeCell ref="G22:I22"/>
-    <mergeCell ref="J17:L17"/>
-    <mergeCell ref="J22:L22"/>
-    <mergeCell ref="G18:I18"/>
-    <mergeCell ref="J18:L18"/>
-    <mergeCell ref="P13:Q13"/>
-    <mergeCell ref="P14:Q14"/>
-    <mergeCell ref="P24:Q24"/>
-    <mergeCell ref="C15:D15"/>
-    <mergeCell ref="C16:D16"/>
-    <mergeCell ref="C23:D23"/>
-    <mergeCell ref="E15:F15"/>
-    <mergeCell ref="E16:F16"/>
-    <mergeCell ref="E23:F23"/>
-    <mergeCell ref="R11:S11"/>
-    <mergeCell ref="R12:S12"/>
-    <mergeCell ref="R13:S13"/>
-    <mergeCell ref="R14:S14"/>
-    <mergeCell ref="R24:S24"/>
-    <mergeCell ref="R15:S15"/>
-    <mergeCell ref="R16:S16"/>
-    <mergeCell ref="R23:S23"/>
-    <mergeCell ref="R17:S17"/>
-    <mergeCell ref="R22:S22"/>
-    <mergeCell ref="R18:S18"/>
-    <mergeCell ref="R19:S19"/>
-    <mergeCell ref="G13:I13"/>
-    <mergeCell ref="J13:L13"/>
-    <mergeCell ref="J14:L14"/>
-    <mergeCell ref="J24:L24"/>
-    <mergeCell ref="M11:O11"/>
-    <mergeCell ref="M12:O12"/>
-    <mergeCell ref="M13:O13"/>
-    <mergeCell ref="M14:O14"/>
-    <mergeCell ref="M24:O24"/>
-    <mergeCell ref="J12:L12"/>
-    <mergeCell ref="J11:L11"/>
-    <mergeCell ref="G15:I15"/>
-    <mergeCell ref="G16:I16"/>
-    <mergeCell ref="G23:I23"/>
-    <mergeCell ref="C13:D13"/>
-    <mergeCell ref="C14:D14"/>
-    <mergeCell ref="C24:D24"/>
-    <mergeCell ref="E11:F11"/>
-    <mergeCell ref="E12:F12"/>
-    <mergeCell ref="C11:D11"/>
-    <mergeCell ref="E13:F13"/>
-    <mergeCell ref="C17:D17"/>
-    <mergeCell ref="C22:D22"/>
-    <mergeCell ref="E17:F17"/>
-    <mergeCell ref="E22:F22"/>
-    <mergeCell ref="C18:D18"/>
-    <mergeCell ref="E18:F18"/>
-    <mergeCell ref="P7:Q7"/>
-    <mergeCell ref="P8:Q8"/>
-    <mergeCell ref="P9:Q9"/>
-    <mergeCell ref="P10:Q10"/>
-    <mergeCell ref="C12:D12"/>
-    <mergeCell ref="P11:Q11"/>
-    <mergeCell ref="P12:Q12"/>
-    <mergeCell ref="J9:L9"/>
-    <mergeCell ref="M9:O9"/>
-    <mergeCell ref="J10:L10"/>
-    <mergeCell ref="M10:O10"/>
-    <mergeCell ref="R6:S6"/>
-    <mergeCell ref="R7:S7"/>
-    <mergeCell ref="R8:S8"/>
-    <mergeCell ref="R9:S9"/>
-    <mergeCell ref="R10:S10"/>
-    <mergeCell ref="J6:L6"/>
-    <mergeCell ref="M6:O6"/>
-    <mergeCell ref="J7:L7"/>
-    <mergeCell ref="M7:O7"/>
-    <mergeCell ref="J8:L8"/>
-    <mergeCell ref="M8:O8"/>
-    <mergeCell ref="P6:Q6"/>
-    <mergeCell ref="G6:I6"/>
-    <mergeCell ref="G7:I7"/>
-    <mergeCell ref="E14:F14"/>
-    <mergeCell ref="E24:F24"/>
-    <mergeCell ref="G8:I8"/>
-    <mergeCell ref="G9:I9"/>
-    <mergeCell ref="G10:I10"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="G11:I11"/>
-    <mergeCell ref="G14:I14"/>
-    <mergeCell ref="G24:I24"/>
-    <mergeCell ref="G12:I12"/>
-    <mergeCell ref="C6:D6"/>
-    <mergeCell ref="C7:D7"/>
-    <mergeCell ref="C8:D8"/>
-    <mergeCell ref="C9:D9"/>
-    <mergeCell ref="C10:D10"/>
-    <mergeCell ref="G5:I5"/>
-    <mergeCell ref="J5:L5"/>
-    <mergeCell ref="M5:O5"/>
-    <mergeCell ref="P5:Q5"/>
-    <mergeCell ref="R5:S5"/>
-    <mergeCell ref="E2:F2"/>
-    <mergeCell ref="E3:F3"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="C2:D2"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="C5:D5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Modify Numbers of Reviews
</commit_message>
<xml_diff>
--- a/Digital_Air_Conditional_Screen/Project Managment/Review Log Sheet/Review Log Sheet.xlsx
+++ b/Digital_Air_Conditional_Screen/Project Managment/Review Log Sheet/Review Log Sheet.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="71">
   <si>
     <t>Project Name:</t>
   </si>
@@ -154,30 +154,9 @@
     <t>Reviewer</t>
   </si>
   <si>
-    <t>Rev_02_05</t>
-  </si>
-  <si>
-    <t>Rev_02_06</t>
-  </si>
-  <si>
-    <t>Rev_02_07</t>
-  </si>
-  <si>
-    <t>Rev_02_08</t>
-  </si>
-  <si>
-    <t>Rev_02_09</t>
-  </si>
-  <si>
-    <t>Rev_02_10</t>
-  </si>
-  <si>
     <t>RTM</t>
   </si>
   <si>
-    <t>Rev_04_04</t>
-  </si>
-  <si>
     <t>Make connection between Tags</t>
   </si>
   <si>
@@ -217,9 +196,6 @@
     <t>Add Tags</t>
   </si>
   <si>
-    <t>Rev_02_11</t>
-  </si>
-  <si>
     <t>CDD DIO</t>
   </si>
   <si>
@@ -227,6 +203,36 @@
   </si>
   <si>
     <t>CDD TS</t>
+  </si>
+  <si>
+    <t>Rev_03_03</t>
+  </si>
+  <si>
+    <t>Rev_04_01</t>
+  </si>
+  <si>
+    <t>Rev_05_01</t>
+  </si>
+  <si>
+    <t>Rev_06_01</t>
+  </si>
+  <si>
+    <t>Rev_07_01</t>
+  </si>
+  <si>
+    <t>Rev_08_01</t>
+  </si>
+  <si>
+    <t>Rev_09_01</t>
+  </si>
+  <si>
+    <t>Rev_10_01</t>
+  </si>
+  <si>
+    <t>Rev_11_01</t>
+  </si>
+  <si>
+    <t>Rev_12_01</t>
   </si>
 </sst>
 </file>
@@ -687,8 +693,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C1:U30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K8" workbookViewId="0">
-      <selection activeCell="R24" sqref="R24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1079,7 +1085,7 @@
     </row>
     <row r="14" spans="3:21" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C14" s="5" t="s">
-        <v>51</v>
+        <v>61</v>
       </c>
       <c r="D14" s="5"/>
       <c r="E14" s="13" t="s">
@@ -1092,7 +1098,7 @@
       <c r="H14" s="5"/>
       <c r="I14" s="5"/>
       <c r="J14" s="5" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="K14" s="5"/>
       <c r="L14" s="5"/>
@@ -1118,7 +1124,7 @@
     </row>
     <row r="15" spans="3:21" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C15" s="5" t="s">
-        <v>44</v>
+        <v>62</v>
       </c>
       <c r="D15" s="5"/>
       <c r="E15" s="13" t="s">
@@ -1126,12 +1132,12 @@
       </c>
       <c r="F15" s="13"/>
       <c r="G15" s="5" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="H15" s="5"/>
       <c r="I15" s="5"/>
       <c r="J15" s="5" t="s">
-        <v>58</v>
+        <v>51</v>
       </c>
       <c r="K15" s="5"/>
       <c r="L15" s="5"/>
@@ -1157,7 +1163,7 @@
     </row>
     <row r="16" spans="3:21" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C16" s="5" t="s">
-        <v>45</v>
+        <v>63</v>
       </c>
       <c r="D16" s="5"/>
       <c r="E16" s="11" t="s">
@@ -1165,12 +1171,12 @@
       </c>
       <c r="F16" s="11"/>
       <c r="G16" s="5" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="H16" s="5"/>
       <c r="I16" s="5"/>
       <c r="J16" s="5" t="s">
-        <v>59</v>
+        <v>52</v>
       </c>
       <c r="K16" s="5"/>
       <c r="L16" s="5"/>
@@ -1196,7 +1202,7 @@
     </row>
     <row r="17" spans="3:21" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C17" s="5" t="s">
-        <v>46</v>
+        <v>64</v>
       </c>
       <c r="D17" s="5"/>
       <c r="E17" s="11" t="s">
@@ -1204,12 +1210,12 @@
       </c>
       <c r="F17" s="11"/>
       <c r="G17" s="5" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="H17" s="5"/>
       <c r="I17" s="5"/>
       <c r="J17" s="5" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
       <c r="K17" s="5"/>
       <c r="L17" s="5"/>
@@ -1235,7 +1241,7 @@
     </row>
     <row r="18" spans="3:21" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C18" s="5" t="s">
-        <v>47</v>
+        <v>65</v>
       </c>
       <c r="D18" s="5"/>
       <c r="E18" s="11" t="s">
@@ -1243,12 +1249,12 @@
       </c>
       <c r="F18" s="11"/>
       <c r="G18" s="5" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="H18" s="5"/>
       <c r="I18" s="5"/>
       <c r="J18" s="5" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="K18" s="5"/>
       <c r="L18" s="5"/>
@@ -1274,7 +1280,7 @@
     </row>
     <row r="19" spans="3:21" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C19" s="5" t="s">
-        <v>48</v>
+        <v>66</v>
       </c>
       <c r="D19" s="5"/>
       <c r="E19" s="11" t="s">
@@ -1282,12 +1288,12 @@
       </c>
       <c r="F19" s="11"/>
       <c r="G19" s="5" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="H19" s="5"/>
       <c r="I19" s="5"/>
       <c r="J19" s="5" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="K19" s="5"/>
       <c r="L19" s="5"/>
@@ -1313,7 +1319,7 @@
     </row>
     <row r="20" spans="3:21" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C20" s="5" t="s">
-        <v>49</v>
+        <v>67</v>
       </c>
       <c r="D20" s="5"/>
       <c r="E20" s="11" t="s">
@@ -1321,12 +1327,12 @@
       </c>
       <c r="F20" s="11"/>
       <c r="G20" s="5" t="s">
-        <v>67</v>
+        <v>59</v>
       </c>
       <c r="H20" s="5"/>
       <c r="I20" s="5"/>
       <c r="J20" s="5" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="K20" s="5"/>
       <c r="L20" s="5"/>
@@ -1352,7 +1358,7 @@
     </row>
     <row r="21" spans="3:21" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C21" s="5" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="D21" s="5"/>
       <c r="E21" s="11" t="s">
@@ -1360,17 +1366,17 @@
       </c>
       <c r="F21" s="11"/>
       <c r="G21" s="5" t="s">
-        <v>68</v>
+        <v>60</v>
       </c>
       <c r="H21" s="5"/>
       <c r="I21" s="5"/>
       <c r="J21" s="5" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="K21" s="5"/>
       <c r="L21" s="5"/>
       <c r="M21" s="5" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="N21" s="5"/>
       <c r="O21" s="5"/>
@@ -1391,7 +1397,7 @@
     </row>
     <row r="22" spans="3:21" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C22" s="5" t="s">
-        <v>47</v>
+        <v>69</v>
       </c>
       <c r="D22" s="5"/>
       <c r="E22" s="11" t="s">
@@ -1399,12 +1405,12 @@
       </c>
       <c r="F22" s="11"/>
       <c r="G22" s="5" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
       <c r="H22" s="5"/>
       <c r="I22" s="5"/>
       <c r="J22" s="5" t="s">
-        <v>62</v>
+        <v>55</v>
       </c>
       <c r="K22" s="5"/>
       <c r="L22" s="5"/>
@@ -1430,7 +1436,7 @@
     </row>
     <row r="23" spans="3:21" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C23" s="5" t="s">
-        <v>51</v>
+        <v>70</v>
       </c>
       <c r="D23" s="5"/>
       <c r="E23" s="13" t="s">
@@ -1438,17 +1444,17 @@
       </c>
       <c r="F23" s="13"/>
       <c r="G23" s="14" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="H23" s="15"/>
       <c r="I23" s="16"/>
       <c r="J23" s="5" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="K23" s="5"/>
       <c r="L23" s="5"/>
       <c r="M23" s="5" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="N23" s="5"/>
       <c r="O23" s="5"/>

</xml_diff>

<commit_message>
Add Review To Make Max & Min Temp and Speed Configurable
</commit_message>
<xml_diff>
--- a/Digital_Air_Conditional_Screen/Project Managment/Review Log Sheet/Review Log Sheet.xlsx
+++ b/Digital_Air_Conditional_Screen/Project Managment/Review Log Sheet/Review Log Sheet.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="74">
   <si>
     <t>Project Name:</t>
   </si>
@@ -233,6 +233,15 @@
   </si>
   <si>
     <t>Rev_12_01</t>
+  </si>
+  <si>
+    <t>Make Max &amp; Min Temp and Speed Configurable by the user</t>
+  </si>
+  <si>
+    <t>Code</t>
+  </si>
+  <si>
+    <t>Rev_13_01</t>
   </si>
 </sst>
 </file>
@@ -372,12 +381,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="14" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -393,13 +396,13 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -410,6 +413,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -691,10 +700,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C1:U30"/>
+  <dimension ref="C1:U33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+    <sheetView tabSelected="1" topLeftCell="L11" workbookViewId="0">
+      <selection activeCell="F27" sqref="F27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -702,29 +711,29 @@
     <col min="5" max="5" width="13" customWidth="1"/>
     <col min="6" max="6" width="13.21875" customWidth="1"/>
     <col min="11" max="11" width="14.109375" customWidth="1"/>
-    <col min="12" max="12" width="15.77734375" customWidth="1"/>
+    <col min="12" max="12" width="26.44140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="3:21" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="3:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C2" s="9" t="s">
+      <c r="C2" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="10"/>
-      <c r="E2" s="7" t="s">
+      <c r="D2" s="8"/>
+      <c r="E2" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="F2" s="8"/>
+      <c r="F2" s="6"/>
     </row>
     <row r="3" spans="3:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C3" s="9" t="s">
+      <c r="C3" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="10"/>
-      <c r="E3" s="7" t="s">
+      <c r="D3" s="8"/>
+      <c r="E3" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="F3" s="8"/>
+      <c r="F3" s="6"/>
     </row>
     <row r="4" spans="3:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C4" s="2"/>
@@ -733,37 +742,37 @@
       <c r="F4" s="2"/>
     </row>
     <row r="5" spans="3:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C5" s="6" t="s">
+      <c r="C5" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="D5" s="6"/>
-      <c r="E5" s="6" t="s">
+      <c r="D5" s="4"/>
+      <c r="E5" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="F5" s="6"/>
-      <c r="G5" s="6" t="s">
+      <c r="F5" s="4"/>
+      <c r="G5" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="H5" s="6"/>
-      <c r="I5" s="6"/>
-      <c r="J5" s="6" t="s">
+      <c r="H5" s="4"/>
+      <c r="I5" s="4"/>
+      <c r="J5" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="K5" s="6"/>
-      <c r="L5" s="6"/>
-      <c r="M5" s="6" t="s">
+      <c r="K5" s="4"/>
+      <c r="L5" s="4"/>
+      <c r="M5" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="N5" s="6"/>
-      <c r="O5" s="6"/>
-      <c r="P5" s="6" t="s">
+      <c r="N5" s="4"/>
+      <c r="O5" s="4"/>
+      <c r="P5" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="Q5" s="6"/>
-      <c r="R5" s="6" t="s">
+      <c r="Q5" s="4"/>
+      <c r="R5" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="S5" s="6"/>
+      <c r="S5" s="4"/>
       <c r="T5" s="3" t="s">
         <v>36</v>
       </c>
@@ -772,37 +781,37 @@
       </c>
     </row>
     <row r="6" spans="3:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C6" s="5" t="s">
+      <c r="C6" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="D6" s="5"/>
-      <c r="E6" s="13" t="s">
+      <c r="D6" s="9"/>
+      <c r="E6" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="F6" s="13"/>
-      <c r="G6" s="5" t="s">
+      <c r="F6" s="10"/>
+      <c r="G6" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="H6" s="5"/>
-      <c r="I6" s="5"/>
-      <c r="J6" s="5" t="s">
+      <c r="H6" s="9"/>
+      <c r="I6" s="9"/>
+      <c r="J6" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="K6" s="5"/>
-      <c r="L6" s="5"/>
-      <c r="M6" s="5" t="s">
+      <c r="K6" s="9"/>
+      <c r="L6" s="9"/>
+      <c r="M6" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="N6" s="5"/>
-      <c r="O6" s="5"/>
-      <c r="P6" s="4">
+      <c r="N6" s="9"/>
+      <c r="O6" s="9"/>
+      <c r="P6" s="11">
         <v>42707</v>
       </c>
-      <c r="Q6" s="5"/>
-      <c r="R6" s="4" t="s">
+      <c r="Q6" s="9"/>
+      <c r="R6" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="S6" s="5"/>
+      <c r="S6" s="9"/>
       <c r="T6" s="1" t="s">
         <v>38</v>
       </c>
@@ -811,37 +820,37 @@
       </c>
     </row>
     <row r="7" spans="3:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C7" s="5" t="s">
+      <c r="C7" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="D7" s="5"/>
-      <c r="E7" s="11" t="s">
+      <c r="D7" s="9"/>
+      <c r="E7" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="F7" s="11"/>
-      <c r="G7" s="5" t="s">
+      <c r="F7" s="15"/>
+      <c r="G7" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="H7" s="5"/>
-      <c r="I7" s="5"/>
-      <c r="J7" s="5" t="s">
+      <c r="H7" s="9"/>
+      <c r="I7" s="9"/>
+      <c r="J7" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="K7" s="5"/>
-      <c r="L7" s="5"/>
-      <c r="M7" s="5" t="s">
+      <c r="K7" s="9"/>
+      <c r="L7" s="9"/>
+      <c r="M7" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="N7" s="5"/>
-      <c r="O7" s="5"/>
-      <c r="P7" s="4">
+      <c r="N7" s="9"/>
+      <c r="O7" s="9"/>
+      <c r="P7" s="11">
         <v>42707</v>
       </c>
-      <c r="Q7" s="5"/>
-      <c r="R7" s="4" t="s">
+      <c r="Q7" s="9"/>
+      <c r="R7" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="S7" s="5"/>
+      <c r="S7" s="9"/>
       <c r="T7" s="1" t="s">
         <v>38</v>
       </c>
@@ -850,37 +859,37 @@
       </c>
     </row>
     <row r="8" spans="3:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C8" s="5" t="s">
+      <c r="C8" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="D8" s="5"/>
-      <c r="E8" s="11" t="s">
+      <c r="D8" s="9"/>
+      <c r="E8" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="F8" s="11"/>
-      <c r="G8" s="5" t="s">
+      <c r="F8" s="15"/>
+      <c r="G8" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="H8" s="5"/>
-      <c r="I8" s="5"/>
-      <c r="J8" s="5" t="s">
+      <c r="H8" s="9"/>
+      <c r="I8" s="9"/>
+      <c r="J8" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="K8" s="5"/>
-      <c r="L8" s="5"/>
-      <c r="M8" s="5" t="s">
+      <c r="K8" s="9"/>
+      <c r="L8" s="9"/>
+      <c r="M8" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="N8" s="5"/>
-      <c r="O8" s="5"/>
-      <c r="P8" s="4">
+      <c r="N8" s="9"/>
+      <c r="O8" s="9"/>
+      <c r="P8" s="11">
         <v>42707</v>
       </c>
-      <c r="Q8" s="5"/>
-      <c r="R8" s="4">
+      <c r="Q8" s="9"/>
+      <c r="R8" s="11">
         <v>42707</v>
       </c>
-      <c r="S8" s="5"/>
+      <c r="S8" s="9"/>
       <c r="T8" s="1" t="s">
         <v>38</v>
       </c>
@@ -889,37 +898,37 @@
       </c>
     </row>
     <row r="9" spans="3:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C9" s="5" t="s">
+      <c r="C9" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="D9" s="5"/>
-      <c r="E9" s="11" t="s">
+      <c r="D9" s="9"/>
+      <c r="E9" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="F9" s="11"/>
-      <c r="G9" s="5" t="s">
+      <c r="F9" s="15"/>
+      <c r="G9" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="H9" s="5"/>
-      <c r="I9" s="5"/>
-      <c r="J9" s="5" t="s">
+      <c r="H9" s="9"/>
+      <c r="I9" s="9"/>
+      <c r="J9" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="K9" s="5"/>
-      <c r="L9" s="5"/>
-      <c r="M9" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="N9" s="5"/>
-      <c r="O9" s="5"/>
-      <c r="P9" s="4">
+      <c r="K9" s="9"/>
+      <c r="L9" s="9"/>
+      <c r="M9" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="N9" s="9"/>
+      <c r="O9" s="9"/>
+      <c r="P9" s="11">
         <v>42707</v>
       </c>
-      <c r="Q9" s="5"/>
-      <c r="R9" s="4" t="s">
+      <c r="Q9" s="9"/>
+      <c r="R9" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="S9" s="5"/>
+      <c r="S9" s="9"/>
       <c r="T9" s="1" t="s">
         <v>38</v>
       </c>
@@ -928,37 +937,37 @@
       </c>
     </row>
     <row r="10" spans="3:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C10" s="5" t="s">
+      <c r="C10" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="D10" s="5"/>
-      <c r="E10" s="13" t="s">
+      <c r="D10" s="9"/>
+      <c r="E10" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="F10" s="13"/>
-      <c r="G10" s="5" t="s">
+      <c r="F10" s="10"/>
+      <c r="G10" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="H10" s="5"/>
-      <c r="I10" s="5"/>
-      <c r="J10" s="5" t="s">
+      <c r="H10" s="9"/>
+      <c r="I10" s="9"/>
+      <c r="J10" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="K10" s="5"/>
-      <c r="L10" s="5"/>
-      <c r="M10" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="N10" s="5"/>
-      <c r="O10" s="5"/>
-      <c r="P10" s="4">
+      <c r="K10" s="9"/>
+      <c r="L10" s="9"/>
+      <c r="M10" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="N10" s="9"/>
+      <c r="O10" s="9"/>
+      <c r="P10" s="11">
         <v>42707</v>
       </c>
-      <c r="Q10" s="5"/>
-      <c r="R10" s="4" t="s">
+      <c r="Q10" s="9"/>
+      <c r="R10" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="S10" s="5"/>
+      <c r="S10" s="9"/>
       <c r="T10" s="1" t="s">
         <v>38</v>
       </c>
@@ -967,37 +976,37 @@
       </c>
     </row>
     <row r="11" spans="3:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C11" s="5" t="s">
+      <c r="C11" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="D11" s="5"/>
-      <c r="E11" s="11" t="s">
+      <c r="D11" s="9"/>
+      <c r="E11" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="F11" s="11"/>
-      <c r="G11" s="5" t="s">
+      <c r="F11" s="15"/>
+      <c r="G11" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="H11" s="5"/>
-      <c r="I11" s="5"/>
-      <c r="J11" s="5" t="s">
+      <c r="H11" s="9"/>
+      <c r="I11" s="9"/>
+      <c r="J11" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="K11" s="5"/>
-      <c r="L11" s="5"/>
-      <c r="M11" s="5" t="s">
+      <c r="K11" s="9"/>
+      <c r="L11" s="9"/>
+      <c r="M11" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="N11" s="5"/>
-      <c r="O11" s="5"/>
-      <c r="P11" s="4">
+      <c r="N11" s="9"/>
+      <c r="O11" s="9"/>
+      <c r="P11" s="11">
         <v>42707</v>
       </c>
-      <c r="Q11" s="5"/>
-      <c r="R11" s="5" t="s">
+      <c r="Q11" s="9"/>
+      <c r="R11" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="S11" s="5"/>
+      <c r="S11" s="9"/>
       <c r="T11" s="1" t="s">
         <v>38</v>
       </c>
@@ -1006,37 +1015,37 @@
       </c>
     </row>
     <row r="12" spans="3:21" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C12" s="5" t="s">
+      <c r="C12" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="D12" s="5"/>
-      <c r="E12" s="13" t="s">
+      <c r="D12" s="9"/>
+      <c r="E12" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="F12" s="13"/>
-      <c r="G12" s="5" t="s">
+      <c r="F12" s="10"/>
+      <c r="G12" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="H12" s="5"/>
-      <c r="I12" s="5"/>
-      <c r="J12" s="5" t="s">
+      <c r="H12" s="9"/>
+      <c r="I12" s="9"/>
+      <c r="J12" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="K12" s="5"/>
-      <c r="L12" s="5"/>
-      <c r="M12" s="5" t="s">
+      <c r="K12" s="9"/>
+      <c r="L12" s="9"/>
+      <c r="M12" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="N12" s="5"/>
-      <c r="O12" s="5"/>
-      <c r="P12" s="4">
+      <c r="N12" s="9"/>
+      <c r="O12" s="9"/>
+      <c r="P12" s="11">
         <v>42707</v>
       </c>
-      <c r="Q12" s="5"/>
-      <c r="R12" s="5" t="s">
+      <c r="Q12" s="9"/>
+      <c r="R12" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="S12" s="5"/>
+      <c r="S12" s="9"/>
       <c r="T12" s="1" t="s">
         <v>38</v>
       </c>
@@ -1045,37 +1054,37 @@
       </c>
     </row>
     <row r="13" spans="3:21" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C13" s="5" t="s">
+      <c r="C13" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="D13" s="5"/>
-      <c r="E13" s="12" t="s">
+      <c r="D13" s="9"/>
+      <c r="E13" s="16" t="s">
         <v>41</v>
       </c>
-      <c r="F13" s="12"/>
-      <c r="G13" s="5" t="s">
+      <c r="F13" s="16"/>
+      <c r="G13" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="H13" s="5"/>
-      <c r="I13" s="5"/>
-      <c r="J13" s="5" t="s">
+      <c r="H13" s="9"/>
+      <c r="I13" s="9"/>
+      <c r="J13" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="K13" s="5"/>
-      <c r="L13" s="5"/>
-      <c r="M13" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="N13" s="5"/>
-      <c r="O13" s="5"/>
-      <c r="P13" s="4">
+      <c r="K13" s="9"/>
+      <c r="L13" s="9"/>
+      <c r="M13" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="N13" s="9"/>
+      <c r="O13" s="9"/>
+      <c r="P13" s="11">
         <v>42404</v>
       </c>
-      <c r="Q13" s="5"/>
-      <c r="R13" s="4">
+      <c r="Q13" s="9"/>
+      <c r="R13" s="11">
         <v>42433</v>
       </c>
-      <c r="S13" s="5"/>
+      <c r="S13" s="9"/>
       <c r="T13" s="1" t="s">
         <v>38</v>
       </c>
@@ -1084,37 +1093,37 @@
       </c>
     </row>
     <row r="14" spans="3:21" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C14" s="5" t="s">
+      <c r="C14" s="9" t="s">
         <v>61</v>
       </c>
-      <c r="D14" s="5"/>
-      <c r="E14" s="13" t="s">
+      <c r="D14" s="9"/>
+      <c r="E14" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="F14" s="13"/>
-      <c r="G14" s="5" t="s">
+      <c r="F14" s="10"/>
+      <c r="G14" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="H14" s="5"/>
-      <c r="I14" s="5"/>
-      <c r="J14" s="5" t="s">
+      <c r="H14" s="9"/>
+      <c r="I14" s="9"/>
+      <c r="J14" s="9" t="s">
         <v>50</v>
       </c>
-      <c r="K14" s="5"/>
-      <c r="L14" s="5"/>
-      <c r="M14" s="5" t="s">
+      <c r="K14" s="9"/>
+      <c r="L14" s="9"/>
+      <c r="M14" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="N14" s="5"/>
-      <c r="O14" s="5"/>
-      <c r="P14" s="4">
+      <c r="N14" s="9"/>
+      <c r="O14" s="9"/>
+      <c r="P14" s="11">
         <v>42404</v>
       </c>
-      <c r="Q14" s="5"/>
-      <c r="R14" s="4">
+      <c r="Q14" s="9"/>
+      <c r="R14" s="11">
         <v>42433</v>
       </c>
-      <c r="S14" s="5"/>
+      <c r="S14" s="9"/>
       <c r="T14" s="1" t="s">
         <v>38</v>
       </c>
@@ -1123,37 +1132,37 @@
       </c>
     </row>
     <row r="15" spans="3:21" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C15" s="5" t="s">
+      <c r="C15" s="9" t="s">
         <v>62</v>
       </c>
-      <c r="D15" s="5"/>
-      <c r="E15" s="13" t="s">
+      <c r="D15" s="9"/>
+      <c r="E15" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="F15" s="13"/>
-      <c r="G15" s="5" t="s">
+      <c r="F15" s="10"/>
+      <c r="G15" s="9" t="s">
         <v>47</v>
       </c>
-      <c r="H15" s="5"/>
-      <c r="I15" s="5"/>
-      <c r="J15" s="5" t="s">
+      <c r="H15" s="9"/>
+      <c r="I15" s="9"/>
+      <c r="J15" s="9" t="s">
         <v>51</v>
       </c>
-      <c r="K15" s="5"/>
-      <c r="L15" s="5"/>
-      <c r="M15" s="5" t="s">
+      <c r="K15" s="9"/>
+      <c r="L15" s="9"/>
+      <c r="M15" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="N15" s="5"/>
-      <c r="O15" s="5"/>
-      <c r="P15" s="4">
+      <c r="N15" s="9"/>
+      <c r="O15" s="9"/>
+      <c r="P15" s="11">
         <v>42433</v>
       </c>
-      <c r="Q15" s="5"/>
-      <c r="R15" s="4">
+      <c r="Q15" s="9"/>
+      <c r="R15" s="11">
         <v>42464</v>
       </c>
-      <c r="S15" s="5"/>
+      <c r="S15" s="9"/>
       <c r="T15" s="1" t="s">
         <v>38</v>
       </c>
@@ -1162,37 +1171,37 @@
       </c>
     </row>
     <row r="16" spans="3:21" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C16" s="5" t="s">
+      <c r="C16" s="9" t="s">
         <v>63</v>
       </c>
-      <c r="D16" s="5"/>
-      <c r="E16" s="11" t="s">
+      <c r="D16" s="9"/>
+      <c r="E16" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="F16" s="11"/>
-      <c r="G16" s="5" t="s">
+      <c r="F16" s="15"/>
+      <c r="G16" s="9" t="s">
         <v>48</v>
       </c>
-      <c r="H16" s="5"/>
-      <c r="I16" s="5"/>
-      <c r="J16" s="5" t="s">
+      <c r="H16" s="9"/>
+      <c r="I16" s="9"/>
+      <c r="J16" s="9" t="s">
         <v>52</v>
       </c>
-      <c r="K16" s="5"/>
-      <c r="L16" s="5"/>
-      <c r="M16" s="5" t="s">
+      <c r="K16" s="9"/>
+      <c r="L16" s="9"/>
+      <c r="M16" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="N16" s="5"/>
-      <c r="O16" s="5"/>
-      <c r="P16" s="4">
+      <c r="N16" s="9"/>
+      <c r="O16" s="9"/>
+      <c r="P16" s="11">
         <v>42433</v>
       </c>
-      <c r="Q16" s="5"/>
-      <c r="R16" s="4">
+      <c r="Q16" s="9"/>
+      <c r="R16" s="11">
         <v>42464</v>
       </c>
-      <c r="S16" s="5"/>
+      <c r="S16" s="9"/>
       <c r="T16" s="1" t="s">
         <v>38</v>
       </c>
@@ -1201,37 +1210,37 @@
       </c>
     </row>
     <row r="17" spans="3:21" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C17" s="5" t="s">
+      <c r="C17" s="9" t="s">
         <v>64</v>
       </c>
-      <c r="D17" s="5"/>
-      <c r="E17" s="11" t="s">
+      <c r="D17" s="9"/>
+      <c r="E17" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="F17" s="11"/>
-      <c r="G17" s="5" t="s">
+      <c r="F17" s="15"/>
+      <c r="G17" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="H17" s="5"/>
-      <c r="I17" s="5"/>
-      <c r="J17" s="5" t="s">
+      <c r="H17" s="9"/>
+      <c r="I17" s="9"/>
+      <c r="J17" s="9" t="s">
         <v>53</v>
       </c>
-      <c r="K17" s="5"/>
-      <c r="L17" s="5"/>
-      <c r="M17" s="5" t="s">
+      <c r="K17" s="9"/>
+      <c r="L17" s="9"/>
+      <c r="M17" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="N17" s="5"/>
-      <c r="O17" s="5"/>
-      <c r="P17" s="4">
+      <c r="N17" s="9"/>
+      <c r="O17" s="9"/>
+      <c r="P17" s="11">
         <v>42494</v>
       </c>
-      <c r="Q17" s="5"/>
-      <c r="R17" s="4">
+      <c r="Q17" s="9"/>
+      <c r="R17" s="11">
         <v>42525</v>
       </c>
-      <c r="S17" s="5"/>
+      <c r="S17" s="9"/>
       <c r="T17" s="1" t="s">
         <v>38</v>
       </c>
@@ -1240,37 +1249,37 @@
       </c>
     </row>
     <row r="18" spans="3:21" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C18" s="5" t="s">
+      <c r="C18" s="9" t="s">
         <v>65</v>
       </c>
-      <c r="D18" s="5"/>
-      <c r="E18" s="11" t="s">
+      <c r="D18" s="9"/>
+      <c r="E18" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="F18" s="11"/>
-      <c r="G18" s="5" t="s">
+      <c r="F18" s="15"/>
+      <c r="G18" s="9" t="s">
         <v>56</v>
       </c>
-      <c r="H18" s="5"/>
-      <c r="I18" s="5"/>
-      <c r="J18" s="5" t="s">
+      <c r="H18" s="9"/>
+      <c r="I18" s="9"/>
+      <c r="J18" s="9" t="s">
         <v>57</v>
       </c>
-      <c r="K18" s="5"/>
-      <c r="L18" s="5"/>
-      <c r="M18" s="5" t="s">
+      <c r="K18" s="9"/>
+      <c r="L18" s="9"/>
+      <c r="M18" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="N18" s="5"/>
-      <c r="O18" s="5"/>
-      <c r="P18" s="4">
+      <c r="N18" s="9"/>
+      <c r="O18" s="9"/>
+      <c r="P18" s="11">
         <v>42525</v>
       </c>
-      <c r="Q18" s="5"/>
-      <c r="R18" s="4">
+      <c r="Q18" s="9"/>
+      <c r="R18" s="11">
         <v>42555</v>
       </c>
-      <c r="S18" s="5"/>
+      <c r="S18" s="9"/>
       <c r="T18" s="1" t="s">
         <v>38</v>
       </c>
@@ -1279,37 +1288,37 @@
       </c>
     </row>
     <row r="19" spans="3:21" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C19" s="5" t="s">
+      <c r="C19" s="9" t="s">
         <v>66</v>
       </c>
-      <c r="D19" s="5"/>
-      <c r="E19" s="11" t="s">
+      <c r="D19" s="9"/>
+      <c r="E19" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="F19" s="11"/>
-      <c r="G19" s="5" t="s">
+      <c r="F19" s="15"/>
+      <c r="G19" s="9" t="s">
         <v>58</v>
       </c>
-      <c r="H19" s="5"/>
-      <c r="I19" s="5"/>
-      <c r="J19" s="5" t="s">
+      <c r="H19" s="9"/>
+      <c r="I19" s="9"/>
+      <c r="J19" s="9" t="s">
         <v>57</v>
       </c>
-      <c r="K19" s="5"/>
-      <c r="L19" s="5"/>
-      <c r="M19" s="5" t="s">
+      <c r="K19" s="9"/>
+      <c r="L19" s="9"/>
+      <c r="M19" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="N19" s="5"/>
-      <c r="O19" s="5"/>
-      <c r="P19" s="4">
+      <c r="N19" s="9"/>
+      <c r="O19" s="9"/>
+      <c r="P19" s="11">
         <v>42525</v>
       </c>
-      <c r="Q19" s="5"/>
-      <c r="R19" s="4">
+      <c r="Q19" s="9"/>
+      <c r="R19" s="11">
         <v>42555</v>
       </c>
-      <c r="S19" s="5"/>
+      <c r="S19" s="9"/>
       <c r="T19" s="1" t="s">
         <v>38</v>
       </c>
@@ -1318,37 +1327,37 @@
       </c>
     </row>
     <row r="20" spans="3:21" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C20" s="5" t="s">
+      <c r="C20" s="9" t="s">
         <v>67</v>
       </c>
-      <c r="D20" s="5"/>
-      <c r="E20" s="11" t="s">
+      <c r="D20" s="9"/>
+      <c r="E20" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="F20" s="11"/>
-      <c r="G20" s="5" t="s">
+      <c r="F20" s="15"/>
+      <c r="G20" s="9" t="s">
         <v>59</v>
       </c>
-      <c r="H20" s="5"/>
-      <c r="I20" s="5"/>
-      <c r="J20" s="5" t="s">
+      <c r="H20" s="9"/>
+      <c r="I20" s="9"/>
+      <c r="J20" s="9" t="s">
         <v>57</v>
       </c>
-      <c r="K20" s="5"/>
-      <c r="L20" s="5"/>
-      <c r="M20" s="5" t="s">
+      <c r="K20" s="9"/>
+      <c r="L20" s="9"/>
+      <c r="M20" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="N20" s="5"/>
-      <c r="O20" s="5"/>
-      <c r="P20" s="4">
+      <c r="N20" s="9"/>
+      <c r="O20" s="9"/>
+      <c r="P20" s="11">
         <v>42525</v>
       </c>
-      <c r="Q20" s="5"/>
-      <c r="R20" s="4">
+      <c r="Q20" s="9"/>
+      <c r="R20" s="11">
         <v>42555</v>
       </c>
-      <c r="S20" s="5"/>
+      <c r="S20" s="9"/>
       <c r="T20" s="1" t="s">
         <v>38</v>
       </c>
@@ -1357,37 +1366,37 @@
       </c>
     </row>
     <row r="21" spans="3:21" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C21" s="5" t="s">
+      <c r="C21" s="9" t="s">
         <v>68</v>
       </c>
-      <c r="D21" s="5"/>
-      <c r="E21" s="11" t="s">
+      <c r="D21" s="9"/>
+      <c r="E21" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="F21" s="11"/>
-      <c r="G21" s="5" t="s">
+      <c r="F21" s="15"/>
+      <c r="G21" s="9" t="s">
         <v>60</v>
       </c>
-      <c r="H21" s="5"/>
-      <c r="I21" s="5"/>
-      <c r="J21" s="5" t="s">
+      <c r="H21" s="9"/>
+      <c r="I21" s="9"/>
+      <c r="J21" s="9" t="s">
         <v>57</v>
       </c>
-      <c r="K21" s="5"/>
-      <c r="L21" s="5"/>
-      <c r="M21" s="5" t="s">
+      <c r="K21" s="9"/>
+      <c r="L21" s="9"/>
+      <c r="M21" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="N21" s="5"/>
-      <c r="O21" s="5"/>
-      <c r="P21" s="4">
+      <c r="N21" s="9"/>
+      <c r="O21" s="9"/>
+      <c r="P21" s="11">
         <v>42525</v>
       </c>
-      <c r="Q21" s="5"/>
-      <c r="R21" s="4">
+      <c r="Q21" s="9"/>
+      <c r="R21" s="11">
         <v>42555</v>
       </c>
-      <c r="S21" s="5"/>
+      <c r="S21" s="9"/>
       <c r="T21" s="1" t="s">
         <v>38</v>
       </c>
@@ -1396,37 +1405,37 @@
       </c>
     </row>
     <row r="22" spans="3:21" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C22" s="5" t="s">
+      <c r="C22" s="9" t="s">
         <v>69</v>
       </c>
-      <c r="D22" s="5"/>
-      <c r="E22" s="11" t="s">
+      <c r="D22" s="9"/>
+      <c r="E22" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="F22" s="11"/>
-      <c r="G22" s="5" t="s">
+      <c r="F22" s="15"/>
+      <c r="G22" s="9" t="s">
         <v>54</v>
       </c>
-      <c r="H22" s="5"/>
-      <c r="I22" s="5"/>
-      <c r="J22" s="5" t="s">
+      <c r="H22" s="9"/>
+      <c r="I22" s="9"/>
+      <c r="J22" s="9" t="s">
         <v>55</v>
       </c>
-      <c r="K22" s="5"/>
-      <c r="L22" s="5"/>
-      <c r="M22" s="5" t="s">
+      <c r="K22" s="9"/>
+      <c r="L22" s="9"/>
+      <c r="M22" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="N22" s="5"/>
-      <c r="O22" s="5"/>
-      <c r="P22" s="4">
+      <c r="N22" s="9"/>
+      <c r="O22" s="9"/>
+      <c r="P22" s="11">
         <v>42525</v>
       </c>
-      <c r="Q22" s="5"/>
-      <c r="R22" s="4">
+      <c r="Q22" s="9"/>
+      <c r="R22" s="11">
         <v>42555</v>
       </c>
-      <c r="S22" s="5"/>
+      <c r="S22" s="9"/>
       <c r="T22" s="1" t="s">
         <v>38</v>
       </c>
@@ -1435,37 +1444,37 @@
       </c>
     </row>
     <row r="23" spans="3:21" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C23" s="5" t="s">
+      <c r="C23" s="9" t="s">
         <v>70</v>
       </c>
-      <c r="D23" s="5"/>
-      <c r="E23" s="13" t="s">
+      <c r="D23" s="9"/>
+      <c r="E23" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="F23" s="13"/>
-      <c r="G23" s="14" t="s">
+      <c r="F23" s="10"/>
+      <c r="G23" s="12" t="s">
         <v>44</v>
       </c>
-      <c r="H23" s="15"/>
-      <c r="I23" s="16"/>
-      <c r="J23" s="5" t="s">
+      <c r="H23" s="13"/>
+      <c r="I23" s="14"/>
+      <c r="J23" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="K23" s="5"/>
-      <c r="L23" s="5"/>
-      <c r="M23" s="5" t="s">
+      <c r="K23" s="9"/>
+      <c r="L23" s="9"/>
+      <c r="M23" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="N23" s="5"/>
-      <c r="O23" s="5"/>
-      <c r="P23" s="4">
+      <c r="N23" s="9"/>
+      <c r="O23" s="9"/>
+      <c r="P23" s="11">
         <v>42555</v>
       </c>
-      <c r="Q23" s="5"/>
-      <c r="R23" s="4">
+      <c r="Q23" s="9"/>
+      <c r="R23" s="11">
         <v>42586</v>
       </c>
-      <c r="S23" s="5"/>
+      <c r="S23" s="9"/>
       <c r="T23" s="1" t="s">
         <v>38</v>
       </c>
@@ -1473,86 +1482,131 @@
         <v>30</v>
       </c>
     </row>
-    <row r="24" spans="3:21" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="25" spans="3:21" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="24" spans="3:21" customFormat="1" ht="15.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C24" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="D24" s="9"/>
+      <c r="E24" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="F24" s="10"/>
+      <c r="G24" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="H24" s="9"/>
+      <c r="I24" s="9"/>
+      <c r="J24" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="K24" s="9"/>
+      <c r="L24" s="9"/>
+      <c r="M24" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="N24" s="9"/>
+      <c r="O24" s="9"/>
+      <c r="P24" s="11">
+        <v>42525</v>
+      </c>
+      <c r="Q24" s="9"/>
+      <c r="R24" s="11">
+        <v>42586</v>
+      </c>
+      <c r="S24" s="9"/>
+      <c r="T24" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="U24" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="25" spans="3:21" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C25" s="9"/>
+      <c r="D25" s="9"/>
+      <c r="E25" s="12"/>
+      <c r="F25" s="13"/>
+      <c r="G25" s="12"/>
+      <c r="H25" s="13"/>
+      <c r="I25" s="14"/>
+      <c r="J25" s="9"/>
+      <c r="K25" s="9"/>
+      <c r="L25" s="9"/>
+      <c r="M25" s="9"/>
+      <c r="N25" s="9"/>
+      <c r="O25" s="9"/>
+      <c r="P25" s="11"/>
+      <c r="Q25" s="9"/>
+      <c r="R25" s="11"/>
+      <c r="S25" s="9"/>
+      <c r="T25" s="1"/>
+      <c r="U25" s="1"/>
+    </row>
     <row r="26" spans="3:21" customFormat="1" x14ac:dyDescent="0.3"/>
     <row r="27" spans="3:21" customFormat="1" x14ac:dyDescent="0.3"/>
     <row r="28" spans="3:21" customFormat="1" x14ac:dyDescent="0.3"/>
     <row r="29" spans="3:21" customFormat="1" x14ac:dyDescent="0.3"/>
     <row r="30" spans="3:21" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="31" spans="3:21" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="32" spans="3:21" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="33" spans="3:21" customFormat="1" x14ac:dyDescent="0.3"/>
   </sheetData>
-  <mergeCells count="137">
-    <mergeCell ref="R5:S5"/>
-    <mergeCell ref="E2:F2"/>
-    <mergeCell ref="E3:F3"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="C2:D2"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="C5:D5"/>
+  <mergeCells count="151">
+    <mergeCell ref="C24:D24"/>
+    <mergeCell ref="E24:F24"/>
+    <mergeCell ref="G24:I24"/>
+    <mergeCell ref="J24:L24"/>
+    <mergeCell ref="M24:O24"/>
+    <mergeCell ref="P24:Q24"/>
+    <mergeCell ref="R24:S24"/>
     <mergeCell ref="C23:D23"/>
     <mergeCell ref="E23:F23"/>
+    <mergeCell ref="G23:I23"/>
     <mergeCell ref="J23:L23"/>
     <mergeCell ref="M23:O23"/>
     <mergeCell ref="P23:Q23"/>
     <mergeCell ref="R23:S23"/>
-    <mergeCell ref="G23:I23"/>
-    <mergeCell ref="C6:D6"/>
-    <mergeCell ref="C7:D7"/>
-    <mergeCell ref="C8:D8"/>
-    <mergeCell ref="C9:D9"/>
-    <mergeCell ref="C10:D10"/>
-    <mergeCell ref="G5:I5"/>
-    <mergeCell ref="J5:L5"/>
-    <mergeCell ref="M5:O5"/>
-    <mergeCell ref="P5:Q5"/>
-    <mergeCell ref="G6:I6"/>
-    <mergeCell ref="G7:I7"/>
-    <mergeCell ref="E14:F14"/>
-    <mergeCell ref="G8:I8"/>
-    <mergeCell ref="G9:I9"/>
-    <mergeCell ref="G10:I10"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="G11:I11"/>
-    <mergeCell ref="G14:I14"/>
-    <mergeCell ref="G12:I12"/>
-    <mergeCell ref="R6:S6"/>
-    <mergeCell ref="R7:S7"/>
-    <mergeCell ref="R8:S8"/>
-    <mergeCell ref="R9:S9"/>
-    <mergeCell ref="R10:S10"/>
-    <mergeCell ref="J6:L6"/>
-    <mergeCell ref="M6:O6"/>
-    <mergeCell ref="J7:L7"/>
-    <mergeCell ref="M7:O7"/>
-    <mergeCell ref="J8:L8"/>
-    <mergeCell ref="M8:O8"/>
-    <mergeCell ref="P6:Q6"/>
-    <mergeCell ref="P7:Q7"/>
-    <mergeCell ref="P8:Q8"/>
-    <mergeCell ref="P9:Q9"/>
-    <mergeCell ref="P10:Q10"/>
-    <mergeCell ref="C12:D12"/>
-    <mergeCell ref="P11:Q11"/>
-    <mergeCell ref="P12:Q12"/>
-    <mergeCell ref="J9:L9"/>
-    <mergeCell ref="M9:O9"/>
-    <mergeCell ref="J10:L10"/>
-    <mergeCell ref="M10:O10"/>
-    <mergeCell ref="J12:L12"/>
-    <mergeCell ref="J11:L11"/>
-    <mergeCell ref="G15:I15"/>
-    <mergeCell ref="G16:I16"/>
-    <mergeCell ref="C13:D13"/>
-    <mergeCell ref="C14:D14"/>
-    <mergeCell ref="E11:F11"/>
-    <mergeCell ref="E12:F12"/>
-    <mergeCell ref="C11:D11"/>
-    <mergeCell ref="E13:F13"/>
-    <mergeCell ref="C17:D17"/>
+    <mergeCell ref="J16:L16"/>
+    <mergeCell ref="C15:D15"/>
+    <mergeCell ref="C16:D16"/>
+    <mergeCell ref="P20:Q20"/>
+    <mergeCell ref="R20:S20"/>
+    <mergeCell ref="C21:D21"/>
+    <mergeCell ref="E21:F21"/>
+    <mergeCell ref="G21:I21"/>
+    <mergeCell ref="J21:L21"/>
+    <mergeCell ref="M21:O21"/>
+    <mergeCell ref="P21:Q21"/>
+    <mergeCell ref="R21:S21"/>
+    <mergeCell ref="C20:D20"/>
+    <mergeCell ref="E20:F20"/>
+    <mergeCell ref="G20:I20"/>
+    <mergeCell ref="J20:L20"/>
+    <mergeCell ref="M20:O20"/>
+    <mergeCell ref="G22:I22"/>
+    <mergeCell ref="J17:L17"/>
+    <mergeCell ref="J22:L22"/>
+    <mergeCell ref="G18:I18"/>
+    <mergeCell ref="J18:L18"/>
+    <mergeCell ref="P13:Q13"/>
+    <mergeCell ref="P14:Q14"/>
+    <mergeCell ref="C19:D19"/>
+    <mergeCell ref="E19:F19"/>
+    <mergeCell ref="G19:I19"/>
+    <mergeCell ref="J19:L19"/>
+    <mergeCell ref="M19:O19"/>
+    <mergeCell ref="P15:Q15"/>
+    <mergeCell ref="P16:Q16"/>
+    <mergeCell ref="M17:O17"/>
+    <mergeCell ref="P17:Q17"/>
+    <mergeCell ref="M22:O22"/>
+    <mergeCell ref="P22:Q22"/>
+    <mergeCell ref="M18:O18"/>
+    <mergeCell ref="P18:Q18"/>
+    <mergeCell ref="P19:Q19"/>
+    <mergeCell ref="M15:O15"/>
+    <mergeCell ref="M16:O16"/>
+    <mergeCell ref="J15:L15"/>
     <mergeCell ref="C22:D22"/>
     <mergeCell ref="E17:F17"/>
     <mergeCell ref="E22:F22"/>
@@ -1577,48 +1631,78 @@
     <mergeCell ref="M12:O12"/>
     <mergeCell ref="M13:O13"/>
     <mergeCell ref="M14:O14"/>
+    <mergeCell ref="G15:I15"/>
+    <mergeCell ref="G16:I16"/>
+    <mergeCell ref="C13:D13"/>
+    <mergeCell ref="C14:D14"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="E12:F12"/>
+    <mergeCell ref="C11:D11"/>
+    <mergeCell ref="E13:F13"/>
+    <mergeCell ref="C17:D17"/>
     <mergeCell ref="G17:I17"/>
-    <mergeCell ref="G22:I22"/>
-    <mergeCell ref="J17:L17"/>
-    <mergeCell ref="J22:L22"/>
-    <mergeCell ref="G18:I18"/>
-    <mergeCell ref="J18:L18"/>
-    <mergeCell ref="P13:Q13"/>
-    <mergeCell ref="P14:Q14"/>
-    <mergeCell ref="C19:D19"/>
-    <mergeCell ref="E19:F19"/>
-    <mergeCell ref="G19:I19"/>
-    <mergeCell ref="J19:L19"/>
-    <mergeCell ref="M19:O19"/>
-    <mergeCell ref="P15:Q15"/>
-    <mergeCell ref="P16:Q16"/>
-    <mergeCell ref="M17:O17"/>
-    <mergeCell ref="P17:Q17"/>
-    <mergeCell ref="M22:O22"/>
-    <mergeCell ref="P22:Q22"/>
-    <mergeCell ref="M18:O18"/>
-    <mergeCell ref="P18:Q18"/>
-    <mergeCell ref="P19:Q19"/>
-    <mergeCell ref="M15:O15"/>
-    <mergeCell ref="M16:O16"/>
-    <mergeCell ref="J15:L15"/>
-    <mergeCell ref="J16:L16"/>
-    <mergeCell ref="C15:D15"/>
-    <mergeCell ref="C16:D16"/>
-    <mergeCell ref="P20:Q20"/>
-    <mergeCell ref="R20:S20"/>
-    <mergeCell ref="C21:D21"/>
-    <mergeCell ref="E21:F21"/>
-    <mergeCell ref="G21:I21"/>
-    <mergeCell ref="J21:L21"/>
-    <mergeCell ref="M21:O21"/>
-    <mergeCell ref="P21:Q21"/>
-    <mergeCell ref="R21:S21"/>
-    <mergeCell ref="C20:D20"/>
-    <mergeCell ref="E20:F20"/>
-    <mergeCell ref="G20:I20"/>
-    <mergeCell ref="J20:L20"/>
-    <mergeCell ref="M20:O20"/>
+    <mergeCell ref="C12:D12"/>
+    <mergeCell ref="P11:Q11"/>
+    <mergeCell ref="P12:Q12"/>
+    <mergeCell ref="J9:L9"/>
+    <mergeCell ref="M9:O9"/>
+    <mergeCell ref="J10:L10"/>
+    <mergeCell ref="M10:O10"/>
+    <mergeCell ref="J12:L12"/>
+    <mergeCell ref="J11:L11"/>
+    <mergeCell ref="R6:S6"/>
+    <mergeCell ref="R7:S7"/>
+    <mergeCell ref="R8:S8"/>
+    <mergeCell ref="R9:S9"/>
+    <mergeCell ref="R10:S10"/>
+    <mergeCell ref="J6:L6"/>
+    <mergeCell ref="M6:O6"/>
+    <mergeCell ref="J7:L7"/>
+    <mergeCell ref="M7:O7"/>
+    <mergeCell ref="J8:L8"/>
+    <mergeCell ref="M8:O8"/>
+    <mergeCell ref="P6:Q6"/>
+    <mergeCell ref="P7:Q7"/>
+    <mergeCell ref="P8:Q8"/>
+    <mergeCell ref="P9:Q9"/>
+    <mergeCell ref="P10:Q10"/>
+    <mergeCell ref="G7:I7"/>
+    <mergeCell ref="E14:F14"/>
+    <mergeCell ref="G8:I8"/>
+    <mergeCell ref="G9:I9"/>
+    <mergeCell ref="G10:I10"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="G11:I11"/>
+    <mergeCell ref="G14:I14"/>
+    <mergeCell ref="G12:I12"/>
+    <mergeCell ref="R5:S5"/>
+    <mergeCell ref="E2:F2"/>
+    <mergeCell ref="E3:F3"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="C25:D25"/>
+    <mergeCell ref="E25:F25"/>
+    <mergeCell ref="J25:L25"/>
+    <mergeCell ref="M25:O25"/>
+    <mergeCell ref="P25:Q25"/>
+    <mergeCell ref="R25:S25"/>
+    <mergeCell ref="G25:I25"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="C7:D7"/>
+    <mergeCell ref="C8:D8"/>
+    <mergeCell ref="C9:D9"/>
+    <mergeCell ref="C10:D10"/>
+    <mergeCell ref="G5:I5"/>
+    <mergeCell ref="J5:L5"/>
+    <mergeCell ref="M5:O5"/>
+    <mergeCell ref="P5:Q5"/>
+    <mergeCell ref="G6:I6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Add Review Add New Test Cases about EEPROM Add CDD Tags for test cases Add Actual hours of Test System
</commit_message>
<xml_diff>
--- a/Digital_Air_Conditional_Screen/Project Managment/Review Log Sheet/Review Log Sheet.xlsx
+++ b/Digital_Air_Conditional_Screen/Project Managment/Review Log Sheet/Review Log Sheet.xlsx
@@ -4,12 +4,12 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="153222"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="12636" windowHeight="6036"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="12636" windowHeight="6288"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="152511"/>
   <oleSize ref="A1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="83">
   <si>
     <t>Project Name:</t>
   </si>
@@ -242,6 +242,33 @@
   </si>
   <si>
     <t>Rev_13_01</t>
+  </si>
+  <si>
+    <t>Rev_12_02</t>
+  </si>
+  <si>
+    <t>Add Tags of CDD</t>
+  </si>
+  <si>
+    <t>Rev_14_01</t>
+  </si>
+  <si>
+    <t>Project Schedule</t>
+  </si>
+  <si>
+    <t>Add Actual time of Test System</t>
+  </si>
+  <si>
+    <t>Rev_11_02</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Add Test Cases for EEPROM </t>
+  </si>
+  <si>
+    <t>Add Tags of CDD to Test Cases</t>
+  </si>
+  <si>
+    <t>Rev_11_03</t>
   </si>
 </sst>
 </file>
@@ -381,21 +408,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -418,6 +430,21 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -700,10 +727,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C1:U33"/>
+  <dimension ref="C1:U37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L11" workbookViewId="0">
-      <selection activeCell="F27" sqref="F27"/>
+    <sheetView tabSelected="1" topLeftCell="I12" workbookViewId="0">
+      <selection activeCell="P26" sqref="P26:Q26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -716,24 +743,24 @@
   <sheetData>
     <row r="1" spans="3:21" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="3:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C2" s="7" t="s">
+      <c r="C2" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="8"/>
-      <c r="E2" s="5" t="s">
+      <c r="D2" s="16"/>
+      <c r="E2" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="F2" s="6"/>
+      <c r="F2" s="14"/>
     </row>
     <row r="3" spans="3:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C3" s="7" t="s">
+      <c r="C3" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="8"/>
-      <c r="E3" s="5" t="s">
+      <c r="D3" s="16"/>
+      <c r="E3" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="F3" s="6"/>
+      <c r="F3" s="14"/>
     </row>
     <row r="4" spans="3:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C4" s="2"/>
@@ -742,37 +769,37 @@
       <c r="F4" s="2"/>
     </row>
     <row r="5" spans="3:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C5" s="4" t="s">
+      <c r="C5" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="D5" s="4"/>
-      <c r="E5" s="4" t="s">
+      <c r="D5" s="12"/>
+      <c r="E5" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="F5" s="4"/>
-      <c r="G5" s="4" t="s">
+      <c r="F5" s="12"/>
+      <c r="G5" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="H5" s="4"/>
-      <c r="I5" s="4"/>
-      <c r="J5" s="4" t="s">
+      <c r="H5" s="12"/>
+      <c r="I5" s="12"/>
+      <c r="J5" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="K5" s="4"/>
-      <c r="L5" s="4"/>
-      <c r="M5" s="4" t="s">
+      <c r="K5" s="12"/>
+      <c r="L5" s="12"/>
+      <c r="M5" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="N5" s="4"/>
-      <c r="O5" s="4"/>
-      <c r="P5" s="4" t="s">
+      <c r="N5" s="12"/>
+      <c r="O5" s="12"/>
+      <c r="P5" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="Q5" s="4"/>
-      <c r="R5" s="4" t="s">
+      <c r="Q5" s="12"/>
+      <c r="R5" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="S5" s="4"/>
+      <c r="S5" s="12"/>
       <c r="T5" s="3" t="s">
         <v>36</v>
       </c>
@@ -781,37 +808,37 @@
       </c>
     </row>
     <row r="6" spans="3:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C6" s="9" t="s">
+      <c r="C6" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="D6" s="9"/>
-      <c r="E6" s="10" t="s">
+      <c r="D6" s="4"/>
+      <c r="E6" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="F6" s="10"/>
-      <c r="G6" s="9" t="s">
+      <c r="F6" s="5"/>
+      <c r="G6" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="H6" s="9"/>
-      <c r="I6" s="9"/>
-      <c r="J6" s="9" t="s">
+      <c r="H6" s="4"/>
+      <c r="I6" s="4"/>
+      <c r="J6" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="K6" s="9"/>
-      <c r="L6" s="9"/>
-      <c r="M6" s="9" t="s">
+      <c r="K6" s="4"/>
+      <c r="L6" s="4"/>
+      <c r="M6" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="N6" s="9"/>
-      <c r="O6" s="9"/>
-      <c r="P6" s="11">
+      <c r="N6" s="4"/>
+      <c r="O6" s="4"/>
+      <c r="P6" s="6">
         <v>42707</v>
       </c>
-      <c r="Q6" s="9"/>
-      <c r="R6" s="11" t="s">
+      <c r="Q6" s="4"/>
+      <c r="R6" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="S6" s="9"/>
+      <c r="S6" s="4"/>
       <c r="T6" s="1" t="s">
         <v>38</v>
       </c>
@@ -820,37 +847,37 @@
       </c>
     </row>
     <row r="7" spans="3:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C7" s="9" t="s">
+      <c r="C7" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="D7" s="9"/>
-      <c r="E7" s="15" t="s">
+      <c r="D7" s="4"/>
+      <c r="E7" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="F7" s="15"/>
-      <c r="G7" s="9" t="s">
+      <c r="F7" s="10"/>
+      <c r="G7" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="H7" s="9"/>
-      <c r="I7" s="9"/>
-      <c r="J7" s="9" t="s">
+      <c r="H7" s="4"/>
+      <c r="I7" s="4"/>
+      <c r="J7" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="K7" s="9"/>
-      <c r="L7" s="9"/>
-      <c r="M7" s="9" t="s">
+      <c r="K7" s="4"/>
+      <c r="L7" s="4"/>
+      <c r="M7" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="N7" s="9"/>
-      <c r="O7" s="9"/>
-      <c r="P7" s="11">
+      <c r="N7" s="4"/>
+      <c r="O7" s="4"/>
+      <c r="P7" s="6">
         <v>42707</v>
       </c>
-      <c r="Q7" s="9"/>
-      <c r="R7" s="11" t="s">
+      <c r="Q7" s="4"/>
+      <c r="R7" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="S7" s="9"/>
+      <c r="S7" s="4"/>
       <c r="T7" s="1" t="s">
         <v>38</v>
       </c>
@@ -859,37 +886,37 @@
       </c>
     </row>
     <row r="8" spans="3:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C8" s="9" t="s">
+      <c r="C8" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="D8" s="9"/>
-      <c r="E8" s="15" t="s">
+      <c r="D8" s="4"/>
+      <c r="E8" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="F8" s="15"/>
-      <c r="G8" s="9" t="s">
+      <c r="F8" s="10"/>
+      <c r="G8" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="H8" s="9"/>
-      <c r="I8" s="9"/>
-      <c r="J8" s="9" t="s">
+      <c r="H8" s="4"/>
+      <c r="I8" s="4"/>
+      <c r="J8" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="K8" s="9"/>
-      <c r="L8" s="9"/>
-      <c r="M8" s="9" t="s">
+      <c r="K8" s="4"/>
+      <c r="L8" s="4"/>
+      <c r="M8" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="N8" s="9"/>
-      <c r="O8" s="9"/>
-      <c r="P8" s="11">
+      <c r="N8" s="4"/>
+      <c r="O8" s="4"/>
+      <c r="P8" s="6">
         <v>42707</v>
       </c>
-      <c r="Q8" s="9"/>
-      <c r="R8" s="11">
+      <c r="Q8" s="4"/>
+      <c r="R8" s="6">
         <v>42707</v>
       </c>
-      <c r="S8" s="9"/>
+      <c r="S8" s="4"/>
       <c r="T8" s="1" t="s">
         <v>38</v>
       </c>
@@ -898,37 +925,37 @@
       </c>
     </row>
     <row r="9" spans="3:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C9" s="9" t="s">
+      <c r="C9" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="D9" s="9"/>
-      <c r="E9" s="15" t="s">
+      <c r="D9" s="4"/>
+      <c r="E9" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="F9" s="15"/>
-      <c r="G9" s="9" t="s">
+      <c r="F9" s="10"/>
+      <c r="G9" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="H9" s="9"/>
-      <c r="I9" s="9"/>
-      <c r="J9" s="9" t="s">
+      <c r="H9" s="4"/>
+      <c r="I9" s="4"/>
+      <c r="J9" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="K9" s="9"/>
-      <c r="L9" s="9"/>
-      <c r="M9" s="9" t="s">
-        <v>30</v>
-      </c>
-      <c r="N9" s="9"/>
-      <c r="O9" s="9"/>
-      <c r="P9" s="11">
+      <c r="K9" s="4"/>
+      <c r="L9" s="4"/>
+      <c r="M9" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="N9" s="4"/>
+      <c r="O9" s="4"/>
+      <c r="P9" s="6">
         <v>42707</v>
       </c>
-      <c r="Q9" s="9"/>
-      <c r="R9" s="11" t="s">
+      <c r="Q9" s="4"/>
+      <c r="R9" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="S9" s="9"/>
+      <c r="S9" s="4"/>
       <c r="T9" s="1" t="s">
         <v>38</v>
       </c>
@@ -937,37 +964,37 @@
       </c>
     </row>
     <row r="10" spans="3:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C10" s="9" t="s">
+      <c r="C10" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="D10" s="9"/>
-      <c r="E10" s="10" t="s">
+      <c r="D10" s="4"/>
+      <c r="E10" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="F10" s="10"/>
-      <c r="G10" s="9" t="s">
+      <c r="F10" s="5"/>
+      <c r="G10" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="H10" s="9"/>
-      <c r="I10" s="9"/>
-      <c r="J10" s="9" t="s">
+      <c r="H10" s="4"/>
+      <c r="I10" s="4"/>
+      <c r="J10" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="K10" s="9"/>
-      <c r="L10" s="9"/>
-      <c r="M10" s="9" t="s">
-        <v>30</v>
-      </c>
-      <c r="N10" s="9"/>
-      <c r="O10" s="9"/>
-      <c r="P10" s="11">
+      <c r="K10" s="4"/>
+      <c r="L10" s="4"/>
+      <c r="M10" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="N10" s="4"/>
+      <c r="O10" s="4"/>
+      <c r="P10" s="6">
         <v>42707</v>
       </c>
-      <c r="Q10" s="9"/>
-      <c r="R10" s="11" t="s">
+      <c r="Q10" s="4"/>
+      <c r="R10" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="S10" s="9"/>
+      <c r="S10" s="4"/>
       <c r="T10" s="1" t="s">
         <v>38</v>
       </c>
@@ -976,37 +1003,37 @@
       </c>
     </row>
     <row r="11" spans="3:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C11" s="9" t="s">
+      <c r="C11" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="D11" s="9"/>
-      <c r="E11" s="15" t="s">
+      <c r="D11" s="4"/>
+      <c r="E11" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="F11" s="15"/>
-      <c r="G11" s="9" t="s">
+      <c r="F11" s="10"/>
+      <c r="G11" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="H11" s="9"/>
-      <c r="I11" s="9"/>
-      <c r="J11" s="9" t="s">
+      <c r="H11" s="4"/>
+      <c r="I11" s="4"/>
+      <c r="J11" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="K11" s="9"/>
-      <c r="L11" s="9"/>
-      <c r="M11" s="9" t="s">
+      <c r="K11" s="4"/>
+      <c r="L11" s="4"/>
+      <c r="M11" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="N11" s="9"/>
-      <c r="O11" s="9"/>
-      <c r="P11" s="11">
+      <c r="N11" s="4"/>
+      <c r="O11" s="4"/>
+      <c r="P11" s="6">
         <v>42707</v>
       </c>
-      <c r="Q11" s="9"/>
-      <c r="R11" s="9" t="s">
+      <c r="Q11" s="4"/>
+      <c r="R11" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="S11" s="9"/>
+      <c r="S11" s="4"/>
       <c r="T11" s="1" t="s">
         <v>38</v>
       </c>
@@ -1015,37 +1042,37 @@
       </c>
     </row>
     <row r="12" spans="3:21" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C12" s="9" t="s">
+      <c r="C12" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="D12" s="9"/>
-      <c r="E12" s="10" t="s">
+      <c r="D12" s="4"/>
+      <c r="E12" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="F12" s="10"/>
-      <c r="G12" s="9" t="s">
+      <c r="F12" s="5"/>
+      <c r="G12" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="H12" s="9"/>
-      <c r="I12" s="9"/>
-      <c r="J12" s="9" t="s">
+      <c r="H12" s="4"/>
+      <c r="I12" s="4"/>
+      <c r="J12" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="K12" s="9"/>
-      <c r="L12" s="9"/>
-      <c r="M12" s="9" t="s">
+      <c r="K12" s="4"/>
+      <c r="L12" s="4"/>
+      <c r="M12" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="N12" s="9"/>
-      <c r="O12" s="9"/>
-      <c r="P12" s="11">
+      <c r="N12" s="4"/>
+      <c r="O12" s="4"/>
+      <c r="P12" s="6">
         <v>42707</v>
       </c>
-      <c r="Q12" s="9"/>
-      <c r="R12" s="9" t="s">
+      <c r="Q12" s="4"/>
+      <c r="R12" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="S12" s="9"/>
+      <c r="S12" s="4"/>
       <c r="T12" s="1" t="s">
         <v>38</v>
       </c>
@@ -1054,37 +1081,37 @@
       </c>
     </row>
     <row r="13" spans="3:21" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C13" s="9" t="s">
+      <c r="C13" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="D13" s="9"/>
-      <c r="E13" s="16" t="s">
+      <c r="D13" s="4"/>
+      <c r="E13" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="F13" s="16"/>
-      <c r="G13" s="9" t="s">
+      <c r="F13" s="11"/>
+      <c r="G13" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="H13" s="9"/>
-      <c r="I13" s="9"/>
-      <c r="J13" s="9" t="s">
+      <c r="H13" s="4"/>
+      <c r="I13" s="4"/>
+      <c r="J13" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="K13" s="9"/>
-      <c r="L13" s="9"/>
-      <c r="M13" s="9" t="s">
-        <v>30</v>
-      </c>
-      <c r="N13" s="9"/>
-      <c r="O13" s="9"/>
-      <c r="P13" s="11">
+      <c r="K13" s="4"/>
+      <c r="L13" s="4"/>
+      <c r="M13" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="N13" s="4"/>
+      <c r="O13" s="4"/>
+      <c r="P13" s="6">
         <v>42404</v>
       </c>
-      <c r="Q13" s="9"/>
-      <c r="R13" s="11">
+      <c r="Q13" s="4"/>
+      <c r="R13" s="6">
         <v>42433</v>
       </c>
-      <c r="S13" s="9"/>
+      <c r="S13" s="4"/>
       <c r="T13" s="1" t="s">
         <v>38</v>
       </c>
@@ -1093,37 +1120,37 @@
       </c>
     </row>
     <row r="14" spans="3:21" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C14" s="9" t="s">
+      <c r="C14" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="D14" s="9"/>
-      <c r="E14" s="10" t="s">
+      <c r="D14" s="4"/>
+      <c r="E14" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="F14" s="10"/>
-      <c r="G14" s="9" t="s">
+      <c r="F14" s="5"/>
+      <c r="G14" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="H14" s="9"/>
-      <c r="I14" s="9"/>
-      <c r="J14" s="9" t="s">
+      <c r="H14" s="4"/>
+      <c r="I14" s="4"/>
+      <c r="J14" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="K14" s="9"/>
-      <c r="L14" s="9"/>
-      <c r="M14" s="9" t="s">
+      <c r="K14" s="4"/>
+      <c r="L14" s="4"/>
+      <c r="M14" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="N14" s="9"/>
-      <c r="O14" s="9"/>
-      <c r="P14" s="11">
+      <c r="N14" s="4"/>
+      <c r="O14" s="4"/>
+      <c r="P14" s="6">
         <v>42404</v>
       </c>
-      <c r="Q14" s="9"/>
-      <c r="R14" s="11">
+      <c r="Q14" s="4"/>
+      <c r="R14" s="6">
         <v>42433</v>
       </c>
-      <c r="S14" s="9"/>
+      <c r="S14" s="4"/>
       <c r="T14" s="1" t="s">
         <v>38</v>
       </c>
@@ -1132,37 +1159,37 @@
       </c>
     </row>
     <row r="15" spans="3:21" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C15" s="9" t="s">
+      <c r="C15" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="D15" s="9"/>
-      <c r="E15" s="10" t="s">
+      <c r="D15" s="4"/>
+      <c r="E15" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="F15" s="10"/>
-      <c r="G15" s="9" t="s">
+      <c r="F15" s="5"/>
+      <c r="G15" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="H15" s="9"/>
-      <c r="I15" s="9"/>
-      <c r="J15" s="9" t="s">
+      <c r="H15" s="4"/>
+      <c r="I15" s="4"/>
+      <c r="J15" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="K15" s="9"/>
-      <c r="L15" s="9"/>
-      <c r="M15" s="9" t="s">
+      <c r="K15" s="4"/>
+      <c r="L15" s="4"/>
+      <c r="M15" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="N15" s="9"/>
-      <c r="O15" s="9"/>
-      <c r="P15" s="11">
+      <c r="N15" s="4"/>
+      <c r="O15" s="4"/>
+      <c r="P15" s="6">
         <v>42433</v>
       </c>
-      <c r="Q15" s="9"/>
-      <c r="R15" s="11">
+      <c r="Q15" s="4"/>
+      <c r="R15" s="6">
         <v>42464</v>
       </c>
-      <c r="S15" s="9"/>
+      <c r="S15" s="4"/>
       <c r="T15" s="1" t="s">
         <v>38</v>
       </c>
@@ -1171,37 +1198,37 @@
       </c>
     </row>
     <row r="16" spans="3:21" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C16" s="9" t="s">
+      <c r="C16" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="D16" s="9"/>
-      <c r="E16" s="15" t="s">
+      <c r="D16" s="4"/>
+      <c r="E16" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="F16" s="15"/>
-      <c r="G16" s="9" t="s">
+      <c r="F16" s="10"/>
+      <c r="G16" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="H16" s="9"/>
-      <c r="I16" s="9"/>
-      <c r="J16" s="9" t="s">
+      <c r="H16" s="4"/>
+      <c r="I16" s="4"/>
+      <c r="J16" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="K16" s="9"/>
-      <c r="L16" s="9"/>
-      <c r="M16" s="9" t="s">
+      <c r="K16" s="4"/>
+      <c r="L16" s="4"/>
+      <c r="M16" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="N16" s="9"/>
-      <c r="O16" s="9"/>
-      <c r="P16" s="11">
+      <c r="N16" s="4"/>
+      <c r="O16" s="4"/>
+      <c r="P16" s="6">
         <v>42433</v>
       </c>
-      <c r="Q16" s="9"/>
-      <c r="R16" s="11">
+      <c r="Q16" s="4"/>
+      <c r="R16" s="6">
         <v>42464</v>
       </c>
-      <c r="S16" s="9"/>
+      <c r="S16" s="4"/>
       <c r="T16" s="1" t="s">
         <v>38</v>
       </c>
@@ -1210,37 +1237,37 @@
       </c>
     </row>
     <row r="17" spans="3:21" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C17" s="9" t="s">
+      <c r="C17" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="D17" s="9"/>
-      <c r="E17" s="15" t="s">
+      <c r="D17" s="4"/>
+      <c r="E17" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="F17" s="15"/>
-      <c r="G17" s="9" t="s">
+      <c r="F17" s="10"/>
+      <c r="G17" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="H17" s="9"/>
-      <c r="I17" s="9"/>
-      <c r="J17" s="9" t="s">
+      <c r="H17" s="4"/>
+      <c r="I17" s="4"/>
+      <c r="J17" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="K17" s="9"/>
-      <c r="L17" s="9"/>
-      <c r="M17" s="9" t="s">
+      <c r="K17" s="4"/>
+      <c r="L17" s="4"/>
+      <c r="M17" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="N17" s="9"/>
-      <c r="O17" s="9"/>
-      <c r="P17" s="11">
+      <c r="N17" s="4"/>
+      <c r="O17" s="4"/>
+      <c r="P17" s="6">
         <v>42494</v>
       </c>
-      <c r="Q17" s="9"/>
-      <c r="R17" s="11">
+      <c r="Q17" s="4"/>
+      <c r="R17" s="6">
         <v>42525</v>
       </c>
-      <c r="S17" s="9"/>
+      <c r="S17" s="4"/>
       <c r="T17" s="1" t="s">
         <v>38</v>
       </c>
@@ -1249,37 +1276,37 @@
       </c>
     </row>
     <row r="18" spans="3:21" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C18" s="9" t="s">
+      <c r="C18" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="D18" s="9"/>
-      <c r="E18" s="15" t="s">
+      <c r="D18" s="4"/>
+      <c r="E18" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="F18" s="15"/>
-      <c r="G18" s="9" t="s">
+      <c r="F18" s="10"/>
+      <c r="G18" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="H18" s="9"/>
-      <c r="I18" s="9"/>
-      <c r="J18" s="9" t="s">
+      <c r="H18" s="4"/>
+      <c r="I18" s="4"/>
+      <c r="J18" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="K18" s="9"/>
-      <c r="L18" s="9"/>
-      <c r="M18" s="9" t="s">
+      <c r="K18" s="4"/>
+      <c r="L18" s="4"/>
+      <c r="M18" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="N18" s="9"/>
-      <c r="O18" s="9"/>
-      <c r="P18" s="11">
+      <c r="N18" s="4"/>
+      <c r="O18" s="4"/>
+      <c r="P18" s="6">
         <v>42525</v>
       </c>
-      <c r="Q18" s="9"/>
-      <c r="R18" s="11">
+      <c r="Q18" s="4"/>
+      <c r="R18" s="6">
         <v>42555</v>
       </c>
-      <c r="S18" s="9"/>
+      <c r="S18" s="4"/>
       <c r="T18" s="1" t="s">
         <v>38</v>
       </c>
@@ -1288,37 +1315,37 @@
       </c>
     </row>
     <row r="19" spans="3:21" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C19" s="9" t="s">
+      <c r="C19" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="D19" s="9"/>
-      <c r="E19" s="15" t="s">
+      <c r="D19" s="4"/>
+      <c r="E19" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="F19" s="15"/>
-      <c r="G19" s="9" t="s">
+      <c r="F19" s="10"/>
+      <c r="G19" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="H19" s="9"/>
-      <c r="I19" s="9"/>
-      <c r="J19" s="9" t="s">
+      <c r="H19" s="4"/>
+      <c r="I19" s="4"/>
+      <c r="J19" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="K19" s="9"/>
-      <c r="L19" s="9"/>
-      <c r="M19" s="9" t="s">
+      <c r="K19" s="4"/>
+      <c r="L19" s="4"/>
+      <c r="M19" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="N19" s="9"/>
-      <c r="O19" s="9"/>
-      <c r="P19" s="11">
+      <c r="N19" s="4"/>
+      <c r="O19" s="4"/>
+      <c r="P19" s="6">
         <v>42525</v>
       </c>
-      <c r="Q19" s="9"/>
-      <c r="R19" s="11">
+      <c r="Q19" s="4"/>
+      <c r="R19" s="6">
         <v>42555</v>
       </c>
-      <c r="S19" s="9"/>
+      <c r="S19" s="4"/>
       <c r="T19" s="1" t="s">
         <v>38</v>
       </c>
@@ -1327,37 +1354,37 @@
       </c>
     </row>
     <row r="20" spans="3:21" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C20" s="9" t="s">
+      <c r="C20" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="D20" s="9"/>
-      <c r="E20" s="15" t="s">
+      <c r="D20" s="4"/>
+      <c r="E20" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="F20" s="15"/>
-      <c r="G20" s="9" t="s">
+      <c r="F20" s="10"/>
+      <c r="G20" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="H20" s="9"/>
-      <c r="I20" s="9"/>
-      <c r="J20" s="9" t="s">
+      <c r="H20" s="4"/>
+      <c r="I20" s="4"/>
+      <c r="J20" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="K20" s="9"/>
-      <c r="L20" s="9"/>
-      <c r="M20" s="9" t="s">
+      <c r="K20" s="4"/>
+      <c r="L20" s="4"/>
+      <c r="M20" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="N20" s="9"/>
-      <c r="O20" s="9"/>
-      <c r="P20" s="11">
+      <c r="N20" s="4"/>
+      <c r="O20" s="4"/>
+      <c r="P20" s="6">
         <v>42525</v>
       </c>
-      <c r="Q20" s="9"/>
-      <c r="R20" s="11">
+      <c r="Q20" s="4"/>
+      <c r="R20" s="6">
         <v>42555</v>
       </c>
-      <c r="S20" s="9"/>
+      <c r="S20" s="4"/>
       <c r="T20" s="1" t="s">
         <v>38</v>
       </c>
@@ -1366,37 +1393,37 @@
       </c>
     </row>
     <row r="21" spans="3:21" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C21" s="9" t="s">
+      <c r="C21" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="D21" s="9"/>
-      <c r="E21" s="15" t="s">
+      <c r="D21" s="4"/>
+      <c r="E21" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="F21" s="15"/>
-      <c r="G21" s="9" t="s">
+      <c r="F21" s="10"/>
+      <c r="G21" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="H21" s="9"/>
-      <c r="I21" s="9"/>
-      <c r="J21" s="9" t="s">
+      <c r="H21" s="4"/>
+      <c r="I21" s="4"/>
+      <c r="J21" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="K21" s="9"/>
-      <c r="L21" s="9"/>
-      <c r="M21" s="9" t="s">
+      <c r="K21" s="4"/>
+      <c r="L21" s="4"/>
+      <c r="M21" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="N21" s="9"/>
-      <c r="O21" s="9"/>
-      <c r="P21" s="11">
+      <c r="N21" s="4"/>
+      <c r="O21" s="4"/>
+      <c r="P21" s="6">
         <v>42525</v>
       </c>
-      <c r="Q21" s="9"/>
-      <c r="R21" s="11">
+      <c r="Q21" s="4"/>
+      <c r="R21" s="6">
         <v>42555</v>
       </c>
-      <c r="S21" s="9"/>
+      <c r="S21" s="4"/>
       <c r="T21" s="1" t="s">
         <v>38</v>
       </c>
@@ -1405,37 +1432,37 @@
       </c>
     </row>
     <row r="22" spans="3:21" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C22" s="9" t="s">
+      <c r="C22" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="D22" s="9"/>
-      <c r="E22" s="15" t="s">
+      <c r="D22" s="4"/>
+      <c r="E22" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="F22" s="15"/>
-      <c r="G22" s="9" t="s">
+      <c r="F22" s="10"/>
+      <c r="G22" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="H22" s="9"/>
-      <c r="I22" s="9"/>
-      <c r="J22" s="9" t="s">
+      <c r="H22" s="4"/>
+      <c r="I22" s="4"/>
+      <c r="J22" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="K22" s="9"/>
-      <c r="L22" s="9"/>
-      <c r="M22" s="9" t="s">
+      <c r="K22" s="4"/>
+      <c r="L22" s="4"/>
+      <c r="M22" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="N22" s="9"/>
-      <c r="O22" s="9"/>
-      <c r="P22" s="11">
+      <c r="N22" s="4"/>
+      <c r="O22" s="4"/>
+      <c r="P22" s="6">
         <v>42525</v>
       </c>
-      <c r="Q22" s="9"/>
-      <c r="R22" s="11">
+      <c r="Q22" s="4"/>
+      <c r="R22" s="6">
         <v>42555</v>
       </c>
-      <c r="S22" s="9"/>
+      <c r="S22" s="4"/>
       <c r="T22" s="1" t="s">
         <v>38</v>
       </c>
@@ -1444,37 +1471,37 @@
       </c>
     </row>
     <row r="23" spans="3:21" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C23" s="9" t="s">
+      <c r="C23" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="D23" s="9"/>
-      <c r="E23" s="10" t="s">
+      <c r="D23" s="4"/>
+      <c r="E23" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="F23" s="10"/>
-      <c r="G23" s="12" t="s">
+      <c r="F23" s="5"/>
+      <c r="G23" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="H23" s="13"/>
-      <c r="I23" s="14"/>
-      <c r="J23" s="9" t="s">
+      <c r="H23" s="8"/>
+      <c r="I23" s="9"/>
+      <c r="J23" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="K23" s="9"/>
-      <c r="L23" s="9"/>
-      <c r="M23" s="9" t="s">
+      <c r="K23" s="4"/>
+      <c r="L23" s="4"/>
+      <c r="M23" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="N23" s="9"/>
-      <c r="O23" s="9"/>
-      <c r="P23" s="11">
+      <c r="N23" s="4"/>
+      <c r="O23" s="4"/>
+      <c r="P23" s="6">
         <v>42555</v>
       </c>
-      <c r="Q23" s="9"/>
-      <c r="R23" s="11">
+      <c r="Q23" s="4"/>
+      <c r="R23" s="6">
         <v>42586</v>
       </c>
-      <c r="S23" s="9"/>
+      <c r="S23" s="4"/>
       <c r="T23" s="1" t="s">
         <v>38</v>
       </c>
@@ -1483,37 +1510,37 @@
       </c>
     </row>
     <row r="24" spans="3:21" customFormat="1" ht="15.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C24" s="9" t="s">
+      <c r="C24" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="D24" s="9"/>
-      <c r="E24" s="10" t="s">
+      <c r="D24" s="4"/>
+      <c r="E24" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="F24" s="10"/>
-      <c r="G24" s="9" t="s">
+      <c r="F24" s="5"/>
+      <c r="G24" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="H24" s="9"/>
-      <c r="I24" s="9"/>
-      <c r="J24" s="9" t="s">
+      <c r="H24" s="4"/>
+      <c r="I24" s="4"/>
+      <c r="J24" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="K24" s="9"/>
-      <c r="L24" s="9"/>
-      <c r="M24" s="9" t="s">
-        <v>30</v>
-      </c>
-      <c r="N24" s="9"/>
-      <c r="O24" s="9"/>
-      <c r="P24" s="11">
+      <c r="K24" s="4"/>
+      <c r="L24" s="4"/>
+      <c r="M24" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="N24" s="4"/>
+      <c r="O24" s="4"/>
+      <c r="P24" s="6">
         <v>42525</v>
       </c>
-      <c r="Q24" s="9"/>
-      <c r="R24" s="11">
+      <c r="Q24" s="4"/>
+      <c r="R24" s="6">
         <v>42586</v>
       </c>
-      <c r="S24" s="9"/>
+      <c r="S24" s="4"/>
       <c r="T24" s="1" t="s">
         <v>38</v>
       </c>
@@ -1521,68 +1548,315 @@
         <v>30</v>
       </c>
     </row>
-    <row r="25" spans="3:21" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C25" s="9"/>
-      <c r="D25" s="9"/>
-      <c r="E25" s="12"/>
-      <c r="F25" s="13"/>
-      <c r="G25" s="12"/>
-      <c r="H25" s="13"/>
-      <c r="I25" s="14"/>
-      <c r="J25" s="9"/>
-      <c r="K25" s="9"/>
-      <c r="L25" s="9"/>
-      <c r="M25" s="9"/>
-      <c r="N25" s="9"/>
-      <c r="O25" s="9"/>
-      <c r="P25" s="11"/>
-      <c r="Q25" s="9"/>
-      <c r="R25" s="11"/>
-      <c r="S25" s="9"/>
-      <c r="T25" s="1"/>
-      <c r="U25" s="1"/>
-    </row>
-    <row r="26" spans="3:21" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="27" spans="3:21" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="28" spans="3:21" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="29" spans="3:21" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="25" spans="3:21" customFormat="1" ht="15.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C25" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="D25" s="4"/>
+      <c r="E25" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="F25" s="5"/>
+      <c r="G25" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="H25" s="8"/>
+      <c r="I25" s="9"/>
+      <c r="J25" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="K25" s="4"/>
+      <c r="L25" s="4"/>
+      <c r="M25" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="N25" s="4"/>
+      <c r="O25" s="4"/>
+      <c r="P25" s="6">
+        <v>42586</v>
+      </c>
+      <c r="Q25" s="4"/>
+      <c r="R25" s="6">
+        <v>42586</v>
+      </c>
+      <c r="S25" s="4"/>
+      <c r="T25" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="U25" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="26" spans="3:21" customFormat="1" ht="15.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C26" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="D26" s="4"/>
+      <c r="E26" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="F26" s="5"/>
+      <c r="G26" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="H26" s="8"/>
+      <c r="I26" s="9"/>
+      <c r="J26" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="K26" s="4"/>
+      <c r="L26" s="4"/>
+      <c r="M26" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="N26" s="4"/>
+      <c r="O26" s="4"/>
+      <c r="P26" s="6">
+        <v>42586</v>
+      </c>
+      <c r="Q26" s="4"/>
+      <c r="R26" s="6">
+        <v>42586</v>
+      </c>
+      <c r="S26" s="4"/>
+      <c r="T26" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="U26" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="27" spans="3:21" customFormat="1" ht="15.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C27" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="D27" s="4"/>
+      <c r="E27" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="F27" s="10"/>
+      <c r="G27" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="H27" s="4"/>
+      <c r="I27" s="4"/>
+      <c r="J27" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="K27" s="4"/>
+      <c r="L27" s="4"/>
+      <c r="M27" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="N27" s="4"/>
+      <c r="O27" s="4"/>
+      <c r="P27" s="6">
+        <v>42586</v>
+      </c>
+      <c r="Q27" s="4"/>
+      <c r="R27" s="6">
+        <v>42586</v>
+      </c>
+      <c r="S27" s="4"/>
+      <c r="T27" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="U27" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="28" spans="3:21" customFormat="1" ht="15.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C28" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="D28" s="4"/>
+      <c r="E28" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="F28" s="10"/>
+      <c r="G28" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="H28" s="4"/>
+      <c r="I28" s="4"/>
+      <c r="J28" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="K28" s="4"/>
+      <c r="L28" s="4"/>
+      <c r="M28" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="N28" s="4"/>
+      <c r="O28" s="4"/>
+      <c r="P28" s="6">
+        <v>42586</v>
+      </c>
+      <c r="Q28" s="4"/>
+      <c r="R28" s="6">
+        <v>42586</v>
+      </c>
+      <c r="S28" s="4"/>
+      <c r="T28" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="U28" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="29" spans="3:21" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C29" s="4"/>
+      <c r="D29" s="4"/>
+      <c r="E29" s="7"/>
+      <c r="F29" s="9"/>
+      <c r="G29" s="7"/>
+      <c r="H29" s="8"/>
+      <c r="I29" s="9"/>
+      <c r="J29" s="4"/>
+      <c r="K29" s="4"/>
+      <c r="L29" s="4"/>
+      <c r="M29" s="4"/>
+      <c r="N29" s="4"/>
+      <c r="O29" s="4"/>
+      <c r="P29" s="6"/>
+      <c r="Q29" s="4"/>
+      <c r="R29" s="6"/>
+      <c r="S29" s="4"/>
+      <c r="T29" s="1"/>
+      <c r="U29" s="1"/>
+    </row>
     <row r="30" spans="3:21" customFormat="1" x14ac:dyDescent="0.3"/>
     <row r="31" spans="3:21" customFormat="1" x14ac:dyDescent="0.3"/>
     <row r="32" spans="3:21" customFormat="1" x14ac:dyDescent="0.3"/>
     <row r="33" spans="3:21" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="34" spans="3:21" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="35" spans="3:21" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="36" spans="3:21" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="37" spans="3:21" customFormat="1" x14ac:dyDescent="0.3"/>
   </sheetData>
-  <mergeCells count="151">
-    <mergeCell ref="C24:D24"/>
-    <mergeCell ref="E24:F24"/>
-    <mergeCell ref="G24:I24"/>
-    <mergeCell ref="J24:L24"/>
-    <mergeCell ref="M24:O24"/>
-    <mergeCell ref="P24:Q24"/>
-    <mergeCell ref="R24:S24"/>
-    <mergeCell ref="C23:D23"/>
-    <mergeCell ref="E23:F23"/>
-    <mergeCell ref="G23:I23"/>
-    <mergeCell ref="J23:L23"/>
-    <mergeCell ref="M23:O23"/>
-    <mergeCell ref="P23:Q23"/>
-    <mergeCell ref="R23:S23"/>
-    <mergeCell ref="J16:L16"/>
-    <mergeCell ref="C15:D15"/>
-    <mergeCell ref="C16:D16"/>
-    <mergeCell ref="P20:Q20"/>
-    <mergeCell ref="R20:S20"/>
-    <mergeCell ref="C21:D21"/>
-    <mergeCell ref="E21:F21"/>
-    <mergeCell ref="G21:I21"/>
-    <mergeCell ref="J21:L21"/>
-    <mergeCell ref="M21:O21"/>
-    <mergeCell ref="P21:Q21"/>
-    <mergeCell ref="R21:S21"/>
-    <mergeCell ref="C20:D20"/>
-    <mergeCell ref="E20:F20"/>
-    <mergeCell ref="G20:I20"/>
-    <mergeCell ref="J20:L20"/>
-    <mergeCell ref="M20:O20"/>
+  <mergeCells count="179">
+    <mergeCell ref="C27:D27"/>
+    <mergeCell ref="E27:F27"/>
+    <mergeCell ref="G27:I27"/>
+    <mergeCell ref="J27:L27"/>
+    <mergeCell ref="M27:O27"/>
+    <mergeCell ref="P27:Q27"/>
+    <mergeCell ref="R27:S27"/>
+    <mergeCell ref="C28:D28"/>
+    <mergeCell ref="E28:F28"/>
+    <mergeCell ref="G28:I28"/>
+    <mergeCell ref="J28:L28"/>
+    <mergeCell ref="M28:O28"/>
+    <mergeCell ref="P28:Q28"/>
+    <mergeCell ref="R28:S28"/>
+    <mergeCell ref="C25:D25"/>
+    <mergeCell ref="E25:F25"/>
+    <mergeCell ref="G25:I25"/>
+    <mergeCell ref="J25:L25"/>
+    <mergeCell ref="M25:O25"/>
+    <mergeCell ref="P25:Q25"/>
+    <mergeCell ref="R25:S25"/>
+    <mergeCell ref="C26:D26"/>
+    <mergeCell ref="E26:F26"/>
+    <mergeCell ref="G26:I26"/>
+    <mergeCell ref="J26:L26"/>
+    <mergeCell ref="M26:O26"/>
+    <mergeCell ref="P26:Q26"/>
+    <mergeCell ref="R26:S26"/>
+    <mergeCell ref="R5:S5"/>
+    <mergeCell ref="E2:F2"/>
+    <mergeCell ref="E3:F3"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="C29:D29"/>
+    <mergeCell ref="E29:F29"/>
+    <mergeCell ref="J29:L29"/>
+    <mergeCell ref="M29:O29"/>
+    <mergeCell ref="P29:Q29"/>
+    <mergeCell ref="R29:S29"/>
+    <mergeCell ref="G29:I29"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="C7:D7"/>
+    <mergeCell ref="C8:D8"/>
+    <mergeCell ref="C9:D9"/>
+    <mergeCell ref="C10:D10"/>
+    <mergeCell ref="G5:I5"/>
+    <mergeCell ref="J5:L5"/>
+    <mergeCell ref="M5:O5"/>
+    <mergeCell ref="P5:Q5"/>
+    <mergeCell ref="G6:I6"/>
+    <mergeCell ref="G7:I7"/>
+    <mergeCell ref="E14:F14"/>
+    <mergeCell ref="G8:I8"/>
+    <mergeCell ref="G9:I9"/>
+    <mergeCell ref="G10:I10"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="G11:I11"/>
+    <mergeCell ref="G14:I14"/>
+    <mergeCell ref="G12:I12"/>
+    <mergeCell ref="P11:Q11"/>
+    <mergeCell ref="P12:Q12"/>
+    <mergeCell ref="J9:L9"/>
+    <mergeCell ref="M9:O9"/>
+    <mergeCell ref="J10:L10"/>
+    <mergeCell ref="M10:O10"/>
+    <mergeCell ref="J12:L12"/>
+    <mergeCell ref="J11:L11"/>
+    <mergeCell ref="R6:S6"/>
+    <mergeCell ref="R7:S7"/>
+    <mergeCell ref="R8:S8"/>
+    <mergeCell ref="R9:S9"/>
+    <mergeCell ref="R10:S10"/>
+    <mergeCell ref="J6:L6"/>
+    <mergeCell ref="M6:O6"/>
+    <mergeCell ref="J7:L7"/>
+    <mergeCell ref="M7:O7"/>
+    <mergeCell ref="J8:L8"/>
+    <mergeCell ref="M8:O8"/>
+    <mergeCell ref="P6:Q6"/>
+    <mergeCell ref="P7:Q7"/>
+    <mergeCell ref="P8:Q8"/>
+    <mergeCell ref="P9:Q9"/>
+    <mergeCell ref="P10:Q10"/>
+    <mergeCell ref="C13:D13"/>
+    <mergeCell ref="C14:D14"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="E12:F12"/>
+    <mergeCell ref="C11:D11"/>
+    <mergeCell ref="E13:F13"/>
+    <mergeCell ref="C17:D17"/>
+    <mergeCell ref="G17:I17"/>
+    <mergeCell ref="C12:D12"/>
+    <mergeCell ref="C22:D22"/>
+    <mergeCell ref="E17:F17"/>
+    <mergeCell ref="E22:F22"/>
+    <mergeCell ref="C18:D18"/>
+    <mergeCell ref="E18:F18"/>
+    <mergeCell ref="E15:F15"/>
+    <mergeCell ref="E16:F16"/>
+    <mergeCell ref="R11:S11"/>
+    <mergeCell ref="R12:S12"/>
+    <mergeCell ref="R13:S13"/>
+    <mergeCell ref="R14:S14"/>
+    <mergeCell ref="R15:S15"/>
+    <mergeCell ref="R16:S16"/>
+    <mergeCell ref="R17:S17"/>
+    <mergeCell ref="R22:S22"/>
+    <mergeCell ref="R18:S18"/>
+    <mergeCell ref="R19:S19"/>
+    <mergeCell ref="G13:I13"/>
+    <mergeCell ref="J13:L13"/>
+    <mergeCell ref="J14:L14"/>
+    <mergeCell ref="M11:O11"/>
+    <mergeCell ref="M12:O12"/>
+    <mergeCell ref="M13:O13"/>
+    <mergeCell ref="M14:O14"/>
     <mergeCell ref="G22:I22"/>
     <mergeCell ref="J17:L17"/>
     <mergeCell ref="J22:L22"/>
@@ -1607,102 +1881,39 @@
     <mergeCell ref="M15:O15"/>
     <mergeCell ref="M16:O16"/>
     <mergeCell ref="J15:L15"/>
-    <mergeCell ref="C22:D22"/>
-    <mergeCell ref="E17:F17"/>
-    <mergeCell ref="E22:F22"/>
-    <mergeCell ref="C18:D18"/>
-    <mergeCell ref="E18:F18"/>
-    <mergeCell ref="E15:F15"/>
-    <mergeCell ref="E16:F16"/>
-    <mergeCell ref="R11:S11"/>
-    <mergeCell ref="R12:S12"/>
-    <mergeCell ref="R13:S13"/>
-    <mergeCell ref="R14:S14"/>
-    <mergeCell ref="R15:S15"/>
-    <mergeCell ref="R16:S16"/>
-    <mergeCell ref="R17:S17"/>
-    <mergeCell ref="R22:S22"/>
-    <mergeCell ref="R18:S18"/>
-    <mergeCell ref="R19:S19"/>
-    <mergeCell ref="G13:I13"/>
-    <mergeCell ref="J13:L13"/>
-    <mergeCell ref="J14:L14"/>
-    <mergeCell ref="M11:O11"/>
-    <mergeCell ref="M12:O12"/>
-    <mergeCell ref="M13:O13"/>
-    <mergeCell ref="M14:O14"/>
+    <mergeCell ref="J16:L16"/>
+    <mergeCell ref="C15:D15"/>
+    <mergeCell ref="C16:D16"/>
+    <mergeCell ref="P20:Q20"/>
+    <mergeCell ref="R20:S20"/>
+    <mergeCell ref="C21:D21"/>
+    <mergeCell ref="E21:F21"/>
+    <mergeCell ref="G21:I21"/>
+    <mergeCell ref="J21:L21"/>
+    <mergeCell ref="M21:O21"/>
+    <mergeCell ref="P21:Q21"/>
+    <mergeCell ref="R21:S21"/>
+    <mergeCell ref="C20:D20"/>
+    <mergeCell ref="E20:F20"/>
+    <mergeCell ref="G20:I20"/>
+    <mergeCell ref="J20:L20"/>
+    <mergeCell ref="M20:O20"/>
     <mergeCell ref="G15:I15"/>
     <mergeCell ref="G16:I16"/>
-    <mergeCell ref="C13:D13"/>
-    <mergeCell ref="C14:D14"/>
-    <mergeCell ref="E11:F11"/>
-    <mergeCell ref="E12:F12"/>
-    <mergeCell ref="C11:D11"/>
-    <mergeCell ref="E13:F13"/>
-    <mergeCell ref="C17:D17"/>
-    <mergeCell ref="G17:I17"/>
-    <mergeCell ref="C12:D12"/>
-    <mergeCell ref="P11:Q11"/>
-    <mergeCell ref="P12:Q12"/>
-    <mergeCell ref="J9:L9"/>
-    <mergeCell ref="M9:O9"/>
-    <mergeCell ref="J10:L10"/>
-    <mergeCell ref="M10:O10"/>
-    <mergeCell ref="J12:L12"/>
-    <mergeCell ref="J11:L11"/>
-    <mergeCell ref="R6:S6"/>
-    <mergeCell ref="R7:S7"/>
-    <mergeCell ref="R8:S8"/>
-    <mergeCell ref="R9:S9"/>
-    <mergeCell ref="R10:S10"/>
-    <mergeCell ref="J6:L6"/>
-    <mergeCell ref="M6:O6"/>
-    <mergeCell ref="J7:L7"/>
-    <mergeCell ref="M7:O7"/>
-    <mergeCell ref="J8:L8"/>
-    <mergeCell ref="M8:O8"/>
-    <mergeCell ref="P6:Q6"/>
-    <mergeCell ref="P7:Q7"/>
-    <mergeCell ref="P8:Q8"/>
-    <mergeCell ref="P9:Q9"/>
-    <mergeCell ref="P10:Q10"/>
-    <mergeCell ref="G7:I7"/>
-    <mergeCell ref="E14:F14"/>
-    <mergeCell ref="G8:I8"/>
-    <mergeCell ref="G9:I9"/>
-    <mergeCell ref="G10:I10"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="G11:I11"/>
-    <mergeCell ref="G14:I14"/>
-    <mergeCell ref="G12:I12"/>
-    <mergeCell ref="R5:S5"/>
-    <mergeCell ref="E2:F2"/>
-    <mergeCell ref="E3:F3"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="C2:D2"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="C5:D5"/>
-    <mergeCell ref="C25:D25"/>
-    <mergeCell ref="E25:F25"/>
-    <mergeCell ref="J25:L25"/>
-    <mergeCell ref="M25:O25"/>
-    <mergeCell ref="P25:Q25"/>
-    <mergeCell ref="R25:S25"/>
-    <mergeCell ref="G25:I25"/>
-    <mergeCell ref="C6:D6"/>
-    <mergeCell ref="C7:D7"/>
-    <mergeCell ref="C8:D8"/>
-    <mergeCell ref="C9:D9"/>
-    <mergeCell ref="C10:D10"/>
-    <mergeCell ref="G5:I5"/>
-    <mergeCell ref="J5:L5"/>
-    <mergeCell ref="M5:O5"/>
-    <mergeCell ref="P5:Q5"/>
-    <mergeCell ref="G6:I6"/>
+    <mergeCell ref="C24:D24"/>
+    <mergeCell ref="E24:F24"/>
+    <mergeCell ref="G24:I24"/>
+    <mergeCell ref="J24:L24"/>
+    <mergeCell ref="M24:O24"/>
+    <mergeCell ref="P24:Q24"/>
+    <mergeCell ref="R24:S24"/>
+    <mergeCell ref="C23:D23"/>
+    <mergeCell ref="E23:F23"/>
+    <mergeCell ref="G23:I23"/>
+    <mergeCell ref="J23:L23"/>
+    <mergeCell ref="M23:O23"/>
+    <mergeCell ref="P23:Q23"/>
+    <mergeCell ref="R23:S23"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Add Tags of Test Cases to RTM
</commit_message>
<xml_diff>
--- a/Digital_Air_Conditional_Screen/Project Managment/Review Log Sheet/Review Log Sheet.xlsx
+++ b/Digital_Air_Conditional_Screen/Project Managment/Review Log Sheet/Review Log Sheet.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="153222"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="12636" windowHeight="6288"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="13284" windowHeight="6036"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="85">
   <si>
     <t>Project Name:</t>
   </si>
@@ -269,6 +269,12 @@
   </si>
   <si>
     <t>Rev_11_03</t>
+  </si>
+  <si>
+    <t>Add Tags of Test Cases</t>
+  </si>
+  <si>
+    <t>Rev_12_03</t>
   </si>
 </sst>
 </file>
@@ -727,10 +733,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C1:U37"/>
+  <dimension ref="C1:U38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I12" workbookViewId="0">
-      <selection activeCell="P26" sqref="P26:Q26"/>
+    <sheetView tabSelected="1" topLeftCell="B15" workbookViewId="0">
+      <selection activeCell="C29" sqref="C29:D29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1612,7 +1618,7 @@
       <c r="N26" s="4"/>
       <c r="O26" s="4"/>
       <c r="P26" s="6">
-        <v>42586</v>
+        <v>42587</v>
       </c>
       <c r="Q26" s="4"/>
       <c r="R26" s="6">
@@ -1704,28 +1710,66 @@
         <v>30</v>
       </c>
     </row>
-    <row r="29" spans="3:21" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C29" s="4"/>
+    <row r="29" spans="3:21" customFormat="1" ht="15.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C29" s="4" t="s">
+        <v>84</v>
+      </c>
       <c r="D29" s="4"/>
-      <c r="E29" s="7"/>
-      <c r="F29" s="9"/>
-      <c r="G29" s="7"/>
+      <c r="E29" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="F29" s="10"/>
+      <c r="G29" s="7" t="s">
+        <v>44</v>
+      </c>
       <c r="H29" s="8"/>
       <c r="I29" s="9"/>
-      <c r="J29" s="4"/>
+      <c r="J29" s="4" t="s">
+        <v>83</v>
+      </c>
       <c r="K29" s="4"/>
       <c r="L29" s="4"/>
-      <c r="M29" s="4"/>
+      <c r="M29" s="4" t="s">
+        <v>30</v>
+      </c>
       <c r="N29" s="4"/>
       <c r="O29" s="4"/>
-      <c r="P29" s="6"/>
+      <c r="P29" s="6">
+        <v>42586</v>
+      </c>
       <c r="Q29" s="4"/>
-      <c r="R29" s="6"/>
+      <c r="R29" s="6">
+        <v>42586</v>
+      </c>
       <c r="S29" s="4"/>
-      <c r="T29" s="1"/>
-      <c r="U29" s="1"/>
-    </row>
-    <row r="30" spans="3:21" customFormat="1" x14ac:dyDescent="0.3"/>
+      <c r="T29" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="U29" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="30" spans="3:21" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C30" s="4"/>
+      <c r="D30" s="4"/>
+      <c r="E30" s="4"/>
+      <c r="F30" s="4"/>
+      <c r="G30" s="7"/>
+      <c r="H30" s="8"/>
+      <c r="I30" s="9"/>
+      <c r="J30" s="4"/>
+      <c r="K30" s="4"/>
+      <c r="L30" s="4"/>
+      <c r="M30" s="4"/>
+      <c r="N30" s="4"/>
+      <c r="O30" s="4"/>
+      <c r="P30" s="6"/>
+      <c r="Q30" s="4"/>
+      <c r="R30" s="6"/>
+      <c r="S30" s="4"/>
+      <c r="T30" s="1"/>
+      <c r="U30" s="1"/>
+    </row>
     <row r="31" spans="3:21" customFormat="1" x14ac:dyDescent="0.3"/>
     <row r="32" spans="3:21" customFormat="1" x14ac:dyDescent="0.3"/>
     <row r="33" spans="3:21" customFormat="1" x14ac:dyDescent="0.3"/>
@@ -1733,8 +1777,16 @@
     <row r="35" spans="3:21" customFormat="1" x14ac:dyDescent="0.3"/>
     <row r="36" spans="3:21" customFormat="1" x14ac:dyDescent="0.3"/>
     <row r="37" spans="3:21" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="38" spans="3:21" customFormat="1" x14ac:dyDescent="0.3"/>
   </sheetData>
-  <mergeCells count="179">
+  <mergeCells count="186">
+    <mergeCell ref="C29:D29"/>
+    <mergeCell ref="E29:F29"/>
+    <mergeCell ref="G29:I29"/>
+    <mergeCell ref="J29:L29"/>
+    <mergeCell ref="M29:O29"/>
+    <mergeCell ref="P29:Q29"/>
+    <mergeCell ref="R29:S29"/>
     <mergeCell ref="C27:D27"/>
     <mergeCell ref="E27:F27"/>
     <mergeCell ref="G27:I27"/>
@@ -1770,13 +1822,13 @@
     <mergeCell ref="C2:D2"/>
     <mergeCell ref="C3:D3"/>
     <mergeCell ref="C5:D5"/>
-    <mergeCell ref="C29:D29"/>
-    <mergeCell ref="E29:F29"/>
-    <mergeCell ref="J29:L29"/>
-    <mergeCell ref="M29:O29"/>
-    <mergeCell ref="P29:Q29"/>
-    <mergeCell ref="R29:S29"/>
-    <mergeCell ref="G29:I29"/>
+    <mergeCell ref="C30:D30"/>
+    <mergeCell ref="E30:F30"/>
+    <mergeCell ref="J30:L30"/>
+    <mergeCell ref="M30:O30"/>
+    <mergeCell ref="P30:Q30"/>
+    <mergeCell ref="R30:S30"/>
+    <mergeCell ref="G30:I30"/>
     <mergeCell ref="C6:D6"/>
     <mergeCell ref="C7:D7"/>
     <mergeCell ref="C8:D8"/>

</xml_diff>